<commit_message>
logsaveRun() now saves actually selected features' ids , instead of progr.
</commit_message>
<xml_diff>
--- a/Tester2.xlsx
+++ b/Tester2.xlsx
@@ -24,7 +24,7 @@
   <calcPr calcId="152511"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId4"/>
-    <pivotCache cacheId="23" r:id="rId5"/>
+    <pivotCache cacheId="16" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -662,11 +662,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1360188448"/>
-        <c:axId val="1360185184"/>
+        <c:axId val="-761442208"/>
+        <c:axId val="-761441120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1360188448"/>
+        <c:axId val="-761442208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -709,7 +709,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1360185184"/>
+        <c:crossAx val="-761441120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -717,7 +717,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1360185184"/>
+        <c:axId val="-761441120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -768,7 +768,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1360188448"/>
+        <c:crossAx val="-761442208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -940,6 +940,47 @@
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="2"/>
@@ -985,6 +1026,47 @@
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -1020,29 +1102,44 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Run!$A$5:$A$7</c:f>
+              <c:f>Run!$A$5:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>133384</c:v>
+                  <c:v>133520</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51192</c:v>
+                  <c:v>134976</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>136024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>136960</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>137196</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>137856</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Run!$B$5:$B$7</c:f>
+              <c:f>Run!$B$5:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1.6516156762295561E-2</c:v>
-                </c:pt>
+                <c:ptCount val="6"/>
                 <c:pt idx="1">
-                  <c:v>1.5990172705072376E-2</c:v>
+                  <c:v>3.3141288456666952E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.515897625147895E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0300426752955627E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1082,39 +1179,49 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Run!$A$5:$A$7</c:f>
+              <c:f>Run!$A$5:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>133384</c:v>
+                  <c:v>133520</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51192</c:v>
+                  <c:v>134976</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>136024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>136960</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>137196</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>137856</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Run!$C$5:$C$7</c:f>
+              <c:f>Run!$C$5:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>3.3760086724508448E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.3842097415652382E-2</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="2">
+                  <c:v>3.883773612943462E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3955207038106339E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.7888838628288173E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2B19-40FC-8792-B72E388B5F83}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1144,29 +1251,44 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Run!$A$5:$A$7</c:f>
+              <c:f>Run!$A$5:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>133384</c:v>
+                  <c:v>133520</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51192</c:v>
+                  <c:v>134976</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>136024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>136960</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>137196</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>137856</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Run!$D$5:$D$7</c:f>
+              <c:f>Run!$D$5:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3.1026730620363974E-2</c:v>
+                  <c:v>3.9946007234232909E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.1092828457186701E-2</c:v>
+                  <c:v>4.5915680880554852E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5688435739856405E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1201,29 +1323,44 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Run!$A$5:$A$7</c:f>
+              <c:f>Run!$A$5:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>133384</c:v>
+                  <c:v>133520</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51192</c:v>
+                  <c:v>134976</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>136024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>136960</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>137196</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>137856</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Run!$E$5:$E$7</c:f>
+              <c:f>Run!$E$5:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3.9405127104566277E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.9329665659002991E-2</c:v>
+                  <c:v>4.2206446785065861E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.2783293378874911E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.2798512137999838E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1239,11 +1376,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1360174848"/>
-        <c:axId val="1360185728"/>
+        <c:axId val="-761439488"/>
+        <c:axId val="-761438944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1360174848"/>
+        <c:axId val="-761439488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1286,7 +1423,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1360185728"/>
+        <c:crossAx val="-761438944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1294,7 +1431,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1360185728"/>
+        <c:axId val="-761438944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1345,7 +1482,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1360174848"/>
+        <c:crossAx val="-761439488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3517,151 +3654,177 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="gcaglion" refreshedDate="43156.486464583337" createdVersion="6" refreshedVersion="5" minRefreshableVersion="3" recordCount="2386586">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="gcaglion" refreshedDate="43156.582428125002" createdVersion="6" refreshedVersion="5" minRefreshableVersion="3" recordCount="71280">
   <cacheSource type="external" connectionId="3"/>
   <cacheFields count="14">
     <cacheField name="PROCESSID" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="204" maxValue="134820" count="136">
-        <n v="204"/>
-        <n v="1372"/>
-        <n v="1540"/>
-        <n v="1932"/>
-        <n v="2792"/>
-        <n v="2800"/>
-        <n v="5692"/>
-        <n v="6648"/>
-        <n v="7100"/>
-        <n v="11232"/>
-        <n v="13364"/>
-        <n v="15080"/>
-        <n v="15344"/>
-        <n v="18280"/>
-        <n v="20184"/>
-        <n v="21748"/>
-        <n v="22992"/>
-        <n v="24204"/>
-        <n v="24348"/>
-        <n v="24416"/>
-        <n v="25652"/>
-        <n v="25896"/>
-        <n v="26432"/>
-        <n v="28712"/>
-        <n v="30920"/>
-        <n v="31956"/>
-        <n v="32516"/>
-        <n v="32652"/>
-        <n v="33304"/>
-        <n v="35652"/>
-        <n v="35660"/>
-        <n v="36028"/>
-        <n v="36100"/>
-        <n v="39232"/>
-        <n v="39408"/>
-        <n v="39864"/>
-        <n v="40760"/>
-        <n v="41964"/>
-        <n v="42156"/>
-        <n v="42856"/>
-        <n v="43124"/>
-        <n v="43192"/>
-        <n v="43512"/>
-        <n v="43552"/>
-        <n v="44444"/>
-        <n v="44892"/>
-        <n v="45140"/>
-        <n v="45516"/>
-        <n v="46436"/>
-        <n v="46736"/>
-        <n v="47272"/>
-        <n v="47364"/>
-        <n v="47540"/>
-        <n v="47620"/>
-        <n v="47720"/>
-        <n v="48080"/>
-        <n v="48108"/>
-        <n v="48148"/>
-        <n v="48340"/>
-        <n v="48408"/>
-        <n v="48420"/>
-        <n v="49400"/>
-        <n v="50480"/>
-        <n v="50516"/>
-        <n v="51192"/>
-        <n v="52916"/>
-        <n v="53196"/>
-        <n v="54012"/>
-        <n v="54912"/>
-        <n v="56864"/>
-        <n v="57572"/>
-        <n v="58820"/>
-        <n v="58908"/>
-        <n v="59188"/>
-        <n v="59232"/>
-        <n v="59520"/>
-        <n v="60516"/>
-        <n v="61520"/>
-        <n v="62200"/>
-        <n v="62252"/>
-        <n v="65600"/>
-        <n v="66576"/>
-        <n v="68172"/>
-        <n v="68332"/>
-        <n v="69212"/>
-        <n v="69736"/>
-        <n v="69744"/>
-        <n v="71240"/>
-        <n v="73656"/>
-        <n v="75272"/>
-        <n v="75860"/>
-        <n v="76352"/>
-        <n v="76784"/>
-        <n v="77892"/>
-        <n v="78280"/>
-        <n v="78540"/>
-        <n v="79928"/>
-        <n v="80584"/>
-        <n v="80640"/>
-        <n v="80664"/>
-        <n v="81520"/>
-        <n v="81684"/>
-        <n v="82796"/>
-        <n v="83400"/>
-        <n v="84052"/>
-        <n v="84076"/>
-        <n v="84436"/>
-        <n v="87852"/>
-        <n v="89780"/>
-        <n v="92856"/>
-        <n v="93268"/>
-        <n v="94568"/>
-        <n v="94576"/>
-        <n v="96972"/>
-        <n v="123572"/>
-        <n v="133312"/>
-        <n v="133384"/>
-        <n v="134664"/>
-        <n v="134708"/>
-        <n v="134752"/>
-        <n v="134820"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="204" maxValue="138212" count="155">
+        <n v="133520"/>
+        <n v="134976"/>
+        <n v="136024"/>
+        <n v="136960"/>
+        <n v="137196"/>
+        <n v="137856"/>
+        <n v="82796" u="1"/>
+        <n v="57572" u="1"/>
+        <n v="1932" u="1"/>
+        <n v="7100" u="1"/>
+        <n v="36028" u="1"/>
+        <n v="84052" u="1"/>
+        <n v="92856" u="1"/>
+        <n v="24204" u="1"/>
+        <n v="44892" u="1"/>
+        <n v="39232" u="1"/>
+        <n v="133912" u="1"/>
+        <n v="43512" u="1"/>
+        <n v="48340" u="1"/>
+        <n v="83400" u="1"/>
+        <n v="15344" u="1"/>
+        <n v="18280" u="1"/>
+        <n v="43552" u="1"/>
+        <n v="54912" u="1"/>
+        <n v="80640" u="1"/>
+        <n v="58908" u="1"/>
+        <n v="44444" u="1"/>
+        <n v="48420" u="1"/>
+        <n v="137152" u="1"/>
+        <n v="24416" u="1"/>
+        <n v="32652" u="1"/>
+        <n v="35660" u="1"/>
+        <n v="46736" u="1"/>
+        <n v="59232" u="1"/>
+        <n v="76784" u="1"/>
+        <n v="15080" u="1"/>
+        <n v="2792" u="1"/>
+        <n v="21748" u="1"/>
+        <n v="47364" u="1"/>
+        <n v="204" u="1"/>
+        <n v="43124" u="1"/>
         <n v="6288" u="1"/>
+        <n v="25896" u="1"/>
+        <n v="73656" u="1"/>
+        <n v="6648" u="1"/>
+        <n v="5692" u="1"/>
+        <n v="62252" u="1"/>
+        <n v="78280" u="1"/>
+        <n v="25652" u="1"/>
+        <n v="33304" u="1"/>
+        <n v="45516" u="1"/>
+        <n v="59188" u="1"/>
+        <n v="133648" u="1"/>
+        <n v="136204" u="1"/>
+        <n v="87852" u="1"/>
+        <n v="1540" u="1"/>
+        <n v="61520" u="1"/>
+        <n v="134172" u="1"/>
+        <n v="134740" u="1"/>
+        <n v="1372" u="1"/>
         <n v="17192" u="1"/>
+        <n v="81684" u="1"/>
+        <n v="134820" u="1"/>
+        <n v="20184" u="1"/>
+        <n v="26432" u="1"/>
+        <n v="39408" u="1"/>
+        <n v="41964" u="1"/>
+        <n v="42856" u="1"/>
+        <n v="68172" u="1"/>
+        <n v="75272" u="1"/>
+        <n v="81520" u="1"/>
+        <n v="84076" u="1"/>
         <n v="2192" u="1"/>
         <n v="22628" u="1"/>
         <n v="78152" u="1"/>
+        <n v="135220" u="1"/>
         <n v="23216" u="1"/>
+        <n v="36100" u="1"/>
+        <n v="58820" u="1"/>
+        <n v="133312" u="1"/>
+        <n v="136152" u="1"/>
+        <n v="54012" u="1"/>
+        <n v="68332" u="1"/>
         <n v="22100" u="1"/>
+        <n v="51192" u="1"/>
+        <n v="80584" u="1"/>
+        <n v="52916" u="1"/>
+        <n v="47540" u="1"/>
+        <n v="48108" u="1"/>
+        <n v="80664" u="1"/>
+        <n v="13364" u="1"/>
+        <n v="22992" u="1"/>
+        <n v="35652" u="1"/>
+        <n v="48148" u="1"/>
+        <n v="84436" u="1"/>
+        <n v="32516" u="1"/>
+        <n v="96972" u="1"/>
+        <n v="47620" u="1"/>
+        <n v="133384" u="1"/>
+        <n v="138212" u="1"/>
+        <n v="50480" u="1"/>
+        <n v="28712" u="1"/>
         <n v="6888" u="1"/>
+        <n v="94576" u="1"/>
+        <n v="137680" u="1"/>
+        <n v="47720" u="1"/>
+        <n v="79928" u="1"/>
+        <n v="69744" u="1"/>
+        <n v="53196" u="1"/>
         <n v="77532" u="1"/>
+        <n v="134752" u="1"/>
         <n v="20708" u="1"/>
+        <n v="47272" u="1"/>
+        <n v="48408" u="1"/>
+        <n v="40760" u="1"/>
+        <n v="66576" u="1"/>
+        <n v="134708" u="1"/>
+        <n v="31956" u="1"/>
+        <n v="69212" u="1"/>
+        <n v="71240" u="1"/>
+        <n v="76352" u="1"/>
+        <n v="134664" u="1"/>
+        <n v="137788" u="1"/>
+        <n v="50516" u="1"/>
+        <n v="65600" u="1"/>
         <n v="77244" u="1"/>
+        <n v="94568" u="1"/>
         <n v="7032" u="1"/>
+        <n v="45140" u="1"/>
+        <n v="49400" u="1"/>
+        <n v="89780" u="1"/>
+        <n v="62200" u="1"/>
+        <n v="77892" u="1"/>
+        <n v="24348" u="1"/>
+        <n v="43192" u="1"/>
+        <n v="60516" u="1"/>
+        <n v="93268" u="1"/>
+        <n v="136120" u="1"/>
         <n v="22512" u="1"/>
+        <n v="69736" u="1"/>
+        <n v="78540" u="1"/>
+        <n v="91320" u="1"/>
+        <n v="2800" u="1"/>
+        <n v="56864" u="1"/>
+        <n v="48080" u="1"/>
         <n v="2412" u="1"/>
         <n v="23536" u="1"/>
+        <n v="30920" u="1"/>
+        <n v="39864" u="1"/>
+        <n v="11232" u="1"/>
+        <n v="42156" u="1"/>
+        <n v="75860" u="1"/>
+        <n v="123572" u="1"/>
+        <n v="46436" u="1"/>
+        <n v="59520" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="THREADID" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="204" maxValue="136040"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="118496" maxValue="136700" count="6">
+        <n v="135128"/>
+        <n v="136568"/>
+        <n v="136700"/>
+        <n v="132888"/>
+        <n v="136312"/>
+        <n v="118496"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="NETPROCESSID" numFmtId="0" sqlType="6">
       <sharedItems containsString="0" containsBlank="1" count="1">
@@ -3674,14 +3837,14 @@
       </sharedItems>
     </cacheField>
     <cacheField name="POS" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="49799"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="5939"/>
     </cacheField>
     <cacheField name="FEATUREID" numFmtId="0" sqlType="6">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="3" count="4">
+        <n v="2"/>
+        <n v="3"/>
         <n v="0"/>
         <n v="1"/>
-        <n v="2"/>
-        <n v="3"/>
       </sharedItems>
     </cacheField>
     <cacheField name="ACTUAL" numFmtId="0" sqlType="6">
@@ -3703,10 +3866,10 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-1.00000023841858" maxValue="1"/>
     </cacheField>
     <cacheField name="PREDICTEDTRS" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-1" maxValue="1"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-0.77474886178970304" maxValue="0.77143287658691395"/>
     </cacheField>
     <cacheField name="ERRORTRS" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="2.00000023841858"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2.12341547012329E-7" maxValue="1.2204825878143299"/>
     </cacheField>
     <cacheField name="BARWIDTH" numFmtId="0" sqlType="6">
       <sharedItems containsString="0" containsBlank="1" count="1">
@@ -4704,147 +4867,166 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
-  <location ref="A3:F7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" fieldListSortAscending="1">
+  <location ref="A3:F11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField axis="axisRow" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="137">
-        <item h="1" x="3"/>
-        <item h="1" m="1" x="123"/>
-        <item h="1" m="1" x="134"/>
-        <item h="1" m="1" x="121"/>
-        <item h="1" m="1" x="128"/>
-        <item h="1" m="1" x="132"/>
-        <item h="1" m="1" x="122"/>
-        <item h="1" m="1" x="130"/>
-        <item h="1" m="1" x="127"/>
-        <item h="1" m="1" x="133"/>
-        <item h="1" m="1" x="124"/>
-        <item h="1" m="1" x="126"/>
-        <item h="1" m="1" x="135"/>
-        <item h="1" x="73"/>
-        <item h="1" m="1" x="131"/>
-        <item h="1" m="1" x="129"/>
-        <item h="1" m="1" x="125"/>
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item h="1" x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="5"/>
-        <item h="1" x="6"/>
-        <item h="1" x="7"/>
-        <item h="1" x="8"/>
-        <item h="1" x="9"/>
-        <item h="1" x="10"/>
-        <item h="1" x="11"/>
-        <item h="1" x="12"/>
-        <item h="1" x="13"/>
-        <item h="1" x="14"/>
-        <item h="1" x="15"/>
-        <item h="1" x="16"/>
-        <item h="1" x="17"/>
-        <item h="1" x="18"/>
-        <item h="1" x="20"/>
-        <item h="1" x="21"/>
-        <item h="1" x="22"/>
-        <item h="1" x="23"/>
-        <item h="1" x="24"/>
-        <item h="1" x="25"/>
-        <item h="1" x="26"/>
-        <item h="1" x="27"/>
-        <item h="1" x="28"/>
-        <item h="1" x="29"/>
-        <item h="1" x="30"/>
-        <item h="1" x="31"/>
-        <item h="1" x="32"/>
-        <item h="1" x="33"/>
-        <item h="1" x="34"/>
-        <item h="1" x="35"/>
-        <item h="1" x="36"/>
-        <item h="1" x="37"/>
-        <item h="1" x="38"/>
-        <item h="1" x="39"/>
-        <item h="1" x="40"/>
-        <item h="1" x="41"/>
-        <item h="1" x="42"/>
-        <item h="1" x="43"/>
-        <item h="1" x="44"/>
-        <item h="1" x="45"/>
-        <item h="1" x="46"/>
-        <item h="1" x="47"/>
-        <item h="1" x="48"/>
-        <item h="1" x="49"/>
-        <item h="1" x="50"/>
-        <item h="1" x="51"/>
-        <item h="1" x="52"/>
-        <item h="1" x="53"/>
-        <item h="1" x="54"/>
-        <item h="1" x="55"/>
-        <item h="1" x="56"/>
-        <item h="1" x="57"/>
-        <item h="1" x="58"/>
-        <item h="1" x="59"/>
-        <item h="1" x="60"/>
-        <item h="1" x="61"/>
-        <item h="1" x="62"/>
-        <item h="1" x="63"/>
-        <item h="1" x="65"/>
-        <item h="1" x="66"/>
-        <item h="1" x="67"/>
-        <item h="1" x="68"/>
-        <item h="1" x="69"/>
-        <item h="1" x="70"/>
-        <item h="1" x="71"/>
-        <item h="1" x="72"/>
-        <item h="1" x="74"/>
-        <item h="1" x="75"/>
-        <item h="1" x="76"/>
-        <item h="1" x="77"/>
-        <item h="1" x="78"/>
-        <item h="1" x="79"/>
-        <item h="1" x="80"/>
-        <item h="1" x="81"/>
-        <item h="1" x="82"/>
-        <item h="1" x="83"/>
-        <item h="1" x="84"/>
-        <item h="1" x="85"/>
-        <item h="1" x="86"/>
-        <item h="1" x="87"/>
-        <item h="1" x="88"/>
-        <item h="1" x="89"/>
-        <item h="1" x="90"/>
-        <item h="1" x="91"/>
-        <item h="1" x="92"/>
-        <item h="1" x="93"/>
-        <item h="1" x="94"/>
-        <item h="1" x="95"/>
-        <item h="1" x="96"/>
-        <item h="1" x="97"/>
-        <item h="1" x="98"/>
-        <item h="1" x="99"/>
-        <item h="1" x="100"/>
-        <item h="1" x="101"/>
-        <item h="1" x="102"/>
-        <item h="1" x="103"/>
-        <item h="1" x="104"/>
-        <item h="1" x="105"/>
-        <item h="1" x="106"/>
-        <item h="1" x="107"/>
-        <item h="1" x="108"/>
-        <item h="1" x="109"/>
-        <item h="1" x="110"/>
-        <item h="1" x="111"/>
-        <item h="1" x="113"/>
-        <item h="1" x="115"/>
-        <item h="1" x="114"/>
-        <item h="1" x="118"/>
-        <item h="1" x="119"/>
-        <item h="1" x="19"/>
-        <item h="1" x="117"/>
-        <item h="1" x="120"/>
-        <item h="1" x="112"/>
-        <item x="116"/>
-        <item x="64"/>
+      <items count="156">
+        <item m="1" x="8"/>
+        <item m="1" x="72"/>
+        <item m="1" x="145"/>
+        <item m="1" x="41"/>
+        <item m="1" x="102"/>
+        <item m="1" x="127"/>
+        <item m="1" x="60"/>
+        <item m="1" x="111"/>
+        <item m="1" x="83"/>
+        <item m="1" x="138"/>
+        <item m="1" x="73"/>
+        <item m="1" x="76"/>
+        <item m="1" x="146"/>
+        <item m="1" x="51"/>
+        <item m="1" x="125"/>
+        <item m="1" x="109"/>
+        <item m="1" x="74"/>
+        <item m="1" x="39"/>
+        <item m="1" x="59"/>
+        <item m="1" x="55"/>
+        <item m="1" x="36"/>
+        <item m="1" x="142"/>
+        <item m="1" x="45"/>
+        <item m="1" x="44"/>
+        <item m="1" x="9"/>
+        <item m="1" x="149"/>
+        <item m="1" x="90"/>
+        <item m="1" x="35"/>
+        <item m="1" x="20"/>
+        <item m="1" x="21"/>
+        <item m="1" x="63"/>
+        <item m="1" x="37"/>
+        <item m="1" x="91"/>
+        <item m="1" x="13"/>
+        <item m="1" x="133"/>
+        <item m="1" x="48"/>
+        <item m="1" x="42"/>
+        <item m="1" x="64"/>
+        <item m="1" x="101"/>
+        <item m="1" x="147"/>
+        <item m="1" x="117"/>
+        <item m="1" x="95"/>
+        <item m="1" x="30"/>
+        <item m="1" x="49"/>
+        <item m="1" x="92"/>
+        <item m="1" x="31"/>
+        <item m="1" x="10"/>
+        <item m="1" x="77"/>
+        <item m="1" x="15"/>
+        <item m="1" x="65"/>
+        <item m="1" x="148"/>
+        <item m="1" x="114"/>
+        <item m="1" x="66"/>
+        <item m="1" x="150"/>
+        <item m="1" x="67"/>
+        <item m="1" x="40"/>
+        <item m="1" x="134"/>
+        <item m="1" x="17"/>
+        <item m="1" x="22"/>
+        <item m="1" x="26"/>
+        <item m="1" x="14"/>
+        <item m="1" x="128"/>
+        <item m="1" x="50"/>
+        <item m="1" x="153"/>
+        <item m="1" x="32"/>
+        <item m="1" x="112"/>
+        <item m="1" x="38"/>
+        <item m="1" x="87"/>
+        <item m="1" x="97"/>
+        <item m="1" x="105"/>
+        <item m="1" x="144"/>
+        <item m="1" x="88"/>
+        <item m="1" x="93"/>
+        <item m="1" x="18"/>
+        <item m="1" x="113"/>
+        <item m="1" x="27"/>
+        <item m="1" x="129"/>
+        <item m="1" x="100"/>
+        <item m="1" x="123"/>
+        <item m="1" x="86"/>
+        <item m="1" x="108"/>
+        <item m="1" x="81"/>
+        <item m="1" x="23"/>
+        <item m="1" x="143"/>
+        <item m="1" x="7"/>
+        <item m="1" x="78"/>
+        <item m="1" x="25"/>
+        <item m="1" x="33"/>
+        <item m="1" x="154"/>
+        <item m="1" x="135"/>
+        <item m="1" x="56"/>
+        <item m="1" x="131"/>
+        <item m="1" x="46"/>
+        <item m="1" x="124"/>
+        <item m="1" x="115"/>
+        <item m="1" x="68"/>
+        <item m="1" x="82"/>
+        <item m="1" x="118"/>
+        <item m="1" x="139"/>
+        <item m="1" x="107"/>
+        <item m="1" x="119"/>
+        <item m="1" x="43"/>
+        <item m="1" x="69"/>
+        <item m="1" x="151"/>
+        <item m="1" x="120"/>
+        <item m="1" x="34"/>
+        <item m="1" x="132"/>
+        <item m="1" x="47"/>
+        <item m="1" x="140"/>
+        <item m="1" x="106"/>
+        <item m="1" x="85"/>
+        <item m="1" x="24"/>
+        <item m="1" x="89"/>
+        <item m="1" x="70"/>
+        <item m="1" x="61"/>
+        <item m="1" x="6"/>
+        <item m="1" x="19"/>
+        <item m="1" x="11"/>
+        <item m="1" x="71"/>
+        <item m="1" x="94"/>
+        <item m="1" x="54"/>
+        <item m="1" x="130"/>
+        <item m="1" x="12"/>
+        <item m="1" x="136"/>
+        <item m="1" x="126"/>
+        <item m="1" x="96"/>
+        <item m="1" x="79"/>
+        <item m="1" x="152"/>
+        <item m="1" x="116"/>
+        <item m="1" x="110"/>
+        <item m="1" x="29"/>
+        <item m="1" x="121"/>
+        <item m="1" x="62"/>
+        <item m="1" x="103"/>
+        <item m="1" x="98"/>
+        <item m="1" x="84"/>
+        <item m="1" x="80"/>
+        <item m="1" x="137"/>
+        <item m="1" x="53"/>
+        <item m="1" x="104"/>
+        <item m="1" x="122"/>
+        <item m="1" x="99"/>
+        <item m="1" x="52"/>
+        <item m="1" x="141"/>
+        <item m="1" x="16"/>
+        <item m="1" x="57"/>
+        <item m="1" x="58"/>
+        <item m="1" x="75"/>
+        <item m="1" x="28"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -4854,10 +5036,10 @@
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
       <items count="5">
+        <item x="2"/>
+        <item x="3"/>
         <item x="0"/>
         <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -4873,12 +5055,24 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="3">
+  <rowItems count="7">
     <i>
-      <x v="134"/>
+      <x v="149"/>
     </i>
     <i>
-      <x v="135"/>
+      <x v="150"/>
+    </i>
+    <i>
+      <x v="151"/>
+    </i>
+    <i>
+      <x v="152"/>
+    </i>
+    <i>
+      <x v="153"/>
+    </i>
+    <i>
+      <x v="154"/>
     </i>
     <i t="grand">
       <x/>
@@ -5190,143 +5384,162 @@
   </pivotTables>
   <data>
     <tabular pivotCacheId="2">
-      <items count="136">
-        <i x="0"/>
-        <i x="1"/>
-        <i x="2"/>
-        <i x="3"/>
-        <i x="4"/>
-        <i x="5"/>
-        <i x="6"/>
-        <i x="7"/>
-        <i x="8"/>
-        <i x="9"/>
-        <i x="10"/>
-        <i x="11"/>
-        <i x="12"/>
-        <i x="13"/>
-        <i x="14"/>
-        <i x="15"/>
-        <i x="16"/>
-        <i x="17"/>
-        <i x="18"/>
-        <i x="19"/>
-        <i x="20"/>
-        <i x="21"/>
-        <i x="22"/>
-        <i x="23"/>
-        <i x="24"/>
-        <i x="25"/>
-        <i x="26"/>
-        <i x="27"/>
-        <i x="28"/>
-        <i x="29"/>
-        <i x="30"/>
-        <i x="31"/>
-        <i x="32"/>
-        <i x="33"/>
-        <i x="34"/>
-        <i x="35"/>
-        <i x="36"/>
-        <i x="37"/>
-        <i x="38"/>
-        <i x="39"/>
-        <i x="40"/>
-        <i x="41"/>
-        <i x="42"/>
-        <i x="43"/>
-        <i x="44"/>
-        <i x="45"/>
-        <i x="46"/>
-        <i x="47"/>
-        <i x="48"/>
-        <i x="49"/>
-        <i x="50"/>
-        <i x="51"/>
-        <i x="52"/>
-        <i x="53"/>
-        <i x="54"/>
-        <i x="55"/>
-        <i x="56"/>
-        <i x="57"/>
-        <i x="58"/>
-        <i x="59"/>
-        <i x="60"/>
-        <i x="61"/>
-        <i x="62"/>
-        <i x="63"/>
-        <i x="64" s="1"/>
-        <i x="65"/>
-        <i x="66"/>
-        <i x="67"/>
-        <i x="68"/>
-        <i x="69"/>
-        <i x="70"/>
-        <i x="71"/>
-        <i x="72"/>
-        <i x="73"/>
-        <i x="74"/>
-        <i x="75"/>
-        <i x="76"/>
-        <i x="77"/>
-        <i x="78"/>
-        <i x="79"/>
-        <i x="80"/>
-        <i x="81"/>
-        <i x="82"/>
-        <i x="83"/>
-        <i x="84"/>
-        <i x="85"/>
-        <i x="86"/>
-        <i x="87"/>
-        <i x="88"/>
-        <i x="89"/>
-        <i x="90"/>
-        <i x="91"/>
-        <i x="92"/>
-        <i x="93"/>
-        <i x="94"/>
-        <i x="95"/>
-        <i x="96"/>
-        <i x="97"/>
-        <i x="98"/>
-        <i x="99"/>
-        <i x="100"/>
-        <i x="101"/>
-        <i x="102"/>
-        <i x="103"/>
-        <i x="104"/>
-        <i x="105"/>
-        <i x="106"/>
-        <i x="107"/>
-        <i x="108"/>
-        <i x="109"/>
-        <i x="110"/>
-        <i x="111"/>
-        <i x="112"/>
-        <i x="113"/>
-        <i x="114"/>
-        <i x="115"/>
-        <i x="116" s="1"/>
-        <i x="117"/>
-        <i x="118"/>
-        <i x="119"/>
-        <i x="120"/>
-        <i x="123" nd="1"/>
-        <i x="134" nd="1"/>
-        <i x="121" nd="1"/>
-        <i x="128" nd="1"/>
-        <i x="132" nd="1"/>
-        <i x="122" nd="1"/>
-        <i x="130" nd="1"/>
-        <i x="127" nd="1"/>
-        <i x="133" nd="1"/>
-        <i x="124" nd="1"/>
-        <i x="126" nd="1"/>
-        <i x="135" nd="1"/>
-        <i x="131" nd="1"/>
-        <i x="129" nd="1"/>
-        <i x="125" nd="1"/>
+      <items count="155">
+        <i x="0" s="1"/>
+        <i x="1" s="1"/>
+        <i x="2" s="1"/>
+        <i x="3" s="1"/>
+        <i x="4" s="1"/>
+        <i x="5" s="1"/>
+        <i x="39" s="1" nd="1"/>
+        <i x="59" s="1" nd="1"/>
+        <i x="55" s="1" nd="1"/>
+        <i x="8" s="1" nd="1"/>
+        <i x="72" s="1" nd="1"/>
+        <i x="145" s="1" nd="1"/>
+        <i x="36" s="1" nd="1"/>
+        <i x="142" s="1" nd="1"/>
+        <i x="45" s="1" nd="1"/>
+        <i x="41" s="1" nd="1"/>
+        <i x="44" s="1" nd="1"/>
+        <i x="102" s="1" nd="1"/>
+        <i x="127" s="1" nd="1"/>
+        <i x="9" s="1" nd="1"/>
+        <i x="149" s="1" nd="1"/>
+        <i x="90" s="1" nd="1"/>
+        <i x="35" s="1" nd="1"/>
+        <i x="20" s="1" nd="1"/>
+        <i x="60" s="1" nd="1"/>
+        <i x="21" s="1" nd="1"/>
+        <i x="63" s="1" nd="1"/>
+        <i x="111" s="1" nd="1"/>
+        <i x="37" s="1" nd="1"/>
+        <i x="83" s="1" nd="1"/>
+        <i x="138" s="1" nd="1"/>
+        <i x="73" s="1" nd="1"/>
+        <i x="91" s="1" nd="1"/>
+        <i x="76" s="1" nd="1"/>
+        <i x="146" s="1" nd="1"/>
+        <i x="13" s="1" nd="1"/>
+        <i x="133" s="1" nd="1"/>
+        <i x="29" s="1" nd="1"/>
+        <i x="48" s="1" nd="1"/>
+        <i x="42" s="1" nd="1"/>
+        <i x="64" s="1" nd="1"/>
+        <i x="101" s="1" nd="1"/>
+        <i x="147" s="1" nd="1"/>
+        <i x="117" s="1" nd="1"/>
+        <i x="95" s="1" nd="1"/>
+        <i x="30" s="1" nd="1"/>
+        <i x="49" s="1" nd="1"/>
+        <i x="92" s="1" nd="1"/>
+        <i x="31" s="1" nd="1"/>
+        <i x="10" s="1" nd="1"/>
+        <i x="77" s="1" nd="1"/>
+        <i x="15" s="1" nd="1"/>
+        <i x="65" s="1" nd="1"/>
+        <i x="148" s="1" nd="1"/>
+        <i x="114" s="1" nd="1"/>
+        <i x="66" s="1" nd="1"/>
+        <i x="150" s="1" nd="1"/>
+        <i x="67" s="1" nd="1"/>
+        <i x="40" s="1" nd="1"/>
+        <i x="134" s="1" nd="1"/>
+        <i x="17" s="1" nd="1"/>
+        <i x="22" s="1" nd="1"/>
+        <i x="26" s="1" nd="1"/>
+        <i x="14" s="1" nd="1"/>
+        <i x="128" s="1" nd="1"/>
+        <i x="50" s="1" nd="1"/>
+        <i x="153" s="1" nd="1"/>
+        <i x="32" s="1" nd="1"/>
+        <i x="112" s="1" nd="1"/>
+        <i x="38" s="1" nd="1"/>
+        <i x="87" s="1" nd="1"/>
+        <i x="97" s="1" nd="1"/>
+        <i x="105" s="1" nd="1"/>
+        <i x="144" s="1" nd="1"/>
+        <i x="88" s="1" nd="1"/>
+        <i x="93" s="1" nd="1"/>
+        <i x="18" s="1" nd="1"/>
+        <i x="113" s="1" nd="1"/>
+        <i x="27" s="1" nd="1"/>
+        <i x="129" s="1" nd="1"/>
+        <i x="100" s="1" nd="1"/>
+        <i x="123" s="1" nd="1"/>
+        <i x="84" s="1" nd="1"/>
+        <i x="86" s="1" nd="1"/>
+        <i x="108" s="1" nd="1"/>
+        <i x="81" s="1" nd="1"/>
+        <i x="23" s="1" nd="1"/>
+        <i x="143" s="1" nd="1"/>
+        <i x="7" s="1" nd="1"/>
+        <i x="78" s="1" nd="1"/>
+        <i x="25" s="1" nd="1"/>
+        <i x="51" s="1" nd="1"/>
+        <i x="33" s="1" nd="1"/>
+        <i x="154" s="1" nd="1"/>
+        <i x="135" s="1" nd="1"/>
+        <i x="56" s="1" nd="1"/>
+        <i x="131" s="1" nd="1"/>
+        <i x="46" s="1" nd="1"/>
+        <i x="124" s="1" nd="1"/>
+        <i x="115" s="1" nd="1"/>
+        <i x="68" s="1" nd="1"/>
+        <i x="82" s="1" nd="1"/>
+        <i x="118" s="1" nd="1"/>
+        <i x="139" s="1" nd="1"/>
+        <i x="107" s="1" nd="1"/>
+        <i x="119" s="1" nd="1"/>
+        <i x="43" s="1" nd="1"/>
+        <i x="69" s="1" nd="1"/>
+        <i x="151" s="1" nd="1"/>
+        <i x="120" s="1" nd="1"/>
+        <i x="34" s="1" nd="1"/>
+        <i x="125" s="1" nd="1"/>
+        <i x="109" s="1" nd="1"/>
+        <i x="132" s="1" nd="1"/>
+        <i x="74" s="1" nd="1"/>
+        <i x="47" s="1" nd="1"/>
+        <i x="140" s="1" nd="1"/>
+        <i x="106" s="1" nd="1"/>
+        <i x="85" s="1" nd="1"/>
+        <i x="24" s="1" nd="1"/>
+        <i x="89" s="1" nd="1"/>
+        <i x="70" s="1" nd="1"/>
+        <i x="61" s="1" nd="1"/>
+        <i x="6" s="1" nd="1"/>
+        <i x="19" s="1" nd="1"/>
+        <i x="11" s="1" nd="1"/>
+        <i x="71" s="1" nd="1"/>
+        <i x="94" s="1" nd="1"/>
+        <i x="54" s="1" nd="1"/>
+        <i x="130" s="1" nd="1"/>
+        <i x="141" s="1" nd="1"/>
+        <i x="12" s="1" nd="1"/>
+        <i x="136" s="1" nd="1"/>
+        <i x="126" s="1" nd="1"/>
+        <i x="103" s="1" nd="1"/>
+        <i x="96" s="1" nd="1"/>
+        <i x="152" s="1" nd="1"/>
+        <i x="79" s="1" nd="1"/>
+        <i x="98" s="1" nd="1"/>
+        <i x="52" s="1" nd="1"/>
+        <i x="16" s="1" nd="1"/>
+        <i x="57" s="1" nd="1"/>
+        <i x="121" s="1" nd="1"/>
+        <i x="116" s="1" nd="1"/>
+        <i x="58" s="1" nd="1"/>
+        <i x="110" s="1" nd="1"/>
+        <i x="62" s="1" nd="1"/>
+        <i x="75" s="1" nd="1"/>
+        <i x="137" s="1" nd="1"/>
+        <i x="80" s="1" nd="1"/>
+        <i x="53" s="1" nd="1"/>
+        <i x="28" s="1" nd="1"/>
+        <i x="104" s="1" nd="1"/>
+        <i x="122" s="1" nd="1"/>
+        <i x="99" s="1" nd="1"/>
       </items>
     </tabular>
   </data>
@@ -5341,7 +5554,7 @@
 
 <file path=xl/slicers/slicer2.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <slicer name="PROCESSID 1" cache="Slicer_PROCESSID1" caption="PROCESSID" startItem="64" rowHeight="241300"/>
+  <slicer name="PROCESSID 1" cache="Slicer_PROCESSID1" caption="PROCESSID" startItem="102" rowHeight="241300"/>
 </slicers>
 </file>
 
@@ -6816,18 +7029,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F7"/>
+  <dimension ref="A3:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="7.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6861,62 +7075,118 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>133384</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1.6516156762295561E-2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>3.3760086724508448E-2</v>
-      </c>
+        <v>133520</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
       <c r="D5" s="1">
-        <v>3.1026730620363974E-2</v>
+        <v>3.9946007234232909E-2</v>
       </c>
       <c r="E5" s="1">
-        <v>3.9405127104566277E-2</v>
+        <v>4.2206446785065861E-2</v>
       </c>
       <c r="F5" s="1">
-        <v>3.0177025302933567E-2</v>
+        <v>4.1076227009649385E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>51192</v>
+        <v>134976</v>
       </c>
       <c r="B6" s="1">
-        <v>1.5990172705072376E-2</v>
-      </c>
-      <c r="C6" s="1">
-        <v>3.3842097415652382E-2</v>
-      </c>
+        <v>3.3141288456666952E-2</v>
+      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1">
-        <v>3.1092828457186701E-2</v>
-      </c>
-      <c r="E6" s="1">
-        <v>3.9329665659002991E-2</v>
-      </c>
+        <v>4.5915680880554852E-2</v>
+      </c>
+      <c r="E6" s="1"/>
       <c r="F6" s="1">
-        <v>3.0063691059228612E-2</v>
+        <v>3.9528484668610898E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="3">
+        <v>136024</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3.515897625147895E-2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3.883773612943462E-2</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1">
+        <v>3.6998356190456785E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>136960</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1">
+        <v>3.3955207038106339E-2</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1">
+        <v>4.2783293378874911E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3.8369250208490628E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>137196</v>
+      </c>
+      <c r="B9" s="1">
+        <v>5.0300426752955627E-3</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1">
+        <v>4.2798512137999838E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2.3914277406647703E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>137856</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1">
+        <v>3.7888838628288173E-2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4.5688435739856405E-2</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1">
+        <v>4.1788637184072289E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1">
-        <v>1.6253164733683968E-2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>3.3801092070080412E-2</v>
-      </c>
-      <c r="D7" s="1">
-        <v>3.1059779538775339E-2</v>
-      </c>
-      <c r="E7" s="1">
-        <v>3.9367396381784638E-2</v>
-      </c>
-      <c r="F7" s="1">
-        <v>3.0120358181081087E-2</v>
+      <c r="B11" s="1">
+        <v>2.4443435794480488E-2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3.6893927265276377E-2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>4.3850041284881389E-2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>4.2596084100646872E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <v>3.6945872111321283E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
successfully run from saved Ws
</commit_message>
<xml_diff>
--- a/Tester2.xlsx
+++ b/Tester2.xlsx
@@ -24,7 +24,7 @@
   <calcPr calcId="152511"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId4"/>
-    <pivotCache cacheId="16" r:id="rId5"/>
+    <pivotCache cacheId="48" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -911,9 +911,6 @@
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -923,7 +920,19 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="none"/>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
@@ -1068,6 +1077,456 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="12"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="13"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="14"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="15"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="16"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="17"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="18"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="19"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="20"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="21"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="22"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="23"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="24"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="25"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="26"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="27"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="28"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="29"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="30"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="31"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="32"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="33"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="34"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -1079,11 +1538,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Run!$B$3:$B$4</c:f>
+              <c:f>Run!$B$3:$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>133100 - 54988</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1098,48 +1557,57 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Run!$A$5:$A$11</c:f>
+              <c:f>Run!$A$6:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>133520</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>134976</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>136024</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>136960</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>137196</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>137856</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Run!$B$5:$B$11</c:f>
+              <c:f>Run!$B$6:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.0951737113021039E-2</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3141288456666952E-2</c:v>
+                  <c:v>5.6764620197591958E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.515897625147895E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0300426752955627E-3</c:v>
+                  <c:v>7.1587257583936068E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.2925817798133253E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1156,11 +1624,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Run!$C$3:$C$4</c:f>
+              <c:f>Run!$C$3:$C$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>139476 - 138304</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1175,192 +1643,57 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Run!$A$5:$A$11</c:f>
+              <c:f>Run!$A$6:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>133520</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>134976</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>136024</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>136960</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>137196</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>137856</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Run!$C$5:$C$11</c:f>
+              <c:f>Run!$C$6:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.0951737113021039E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.6764620197591958E-2</c:v>
+                </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.883773612943462E-2</c:v>
+                  <c:v>7.1587257583936068E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3955207038106339E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.7888838628288173E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Run!$D$3:$D$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Run!$A$5:$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>133520</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>134976</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>136024</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>136960</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>137196</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>137856</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Run!$D$5:$D$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>3.9946007234232909E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.5915680880554852E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.5688435739856405E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Run!$E$3:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Run!$A$5:$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>133520</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>134976</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>136024</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>136960</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>137196</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>137856</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Run!$E$5:$E$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>4.2206446785065861E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.2783293378874911E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.2798512137999838E-2</c:v>
+                  <c:v>8.2925817798133253E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1375,6 +1708,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="-761439488"/>
         <c:axId val="-761438944"/>
@@ -2743,16 +3077,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>33337</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>61912</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>338137</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>366712</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2779,8 +3113,8 @@
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -3654,37 +3988,40 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="gcaglion" refreshedDate="43156.582428125002" createdVersion="6" refreshedVersion="5" minRefreshableVersion="3" recordCount="71280">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="gcaglion" refreshedDate="43156.838012384258" createdVersion="6" refreshedVersion="5" minRefreshableVersion="3" recordCount="4320">
   <cacheSource type="external" connectionId="3"/>
   <cacheFields count="14">
     <cacheField name="PROCESSID" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="204" maxValue="138212" count="155">
-        <n v="133520"/>
-        <n v="134976"/>
-        <n v="136024"/>
-        <n v="136960"/>
-        <n v="137196"/>
-        <n v="137856"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="204" maxValue="139476" count="177">
+        <n v="133100"/>
+        <n v="139476"/>
         <n v="82796" u="1"/>
         <n v="57572" u="1"/>
+        <n v="134852" u="1"/>
         <n v="1932" u="1"/>
         <n v="7100" u="1"/>
         <n v="36028" u="1"/>
         <n v="84052" u="1"/>
         <n v="92856" u="1"/>
+        <n v="137000" u="1"/>
+        <n v="136024" u="1"/>
         <n v="24204" u="1"/>
         <n v="44892" u="1"/>
+        <n v="134400" u="1"/>
         <n v="39232" u="1"/>
         <n v="133912" u="1"/>
         <n v="43512" u="1"/>
         <n v="48340" u="1"/>
         <n v="83400" u="1"/>
+        <n v="38136" u="1"/>
+        <n v="137196" u="1"/>
         <n v="15344" u="1"/>
         <n v="18280" u="1"/>
         <n v="43552" u="1"/>
         <n v="54912" u="1"/>
         <n v="80640" u="1"/>
         <n v="58908" u="1"/>
+        <n v="138208" u="1"/>
         <n v="44444" u="1"/>
         <n v="48420" u="1"/>
         <n v="137152" u="1"/>
@@ -3698,11 +4035,16 @@
         <n v="2792" u="1"/>
         <n v="21748" u="1"/>
         <n v="47364" u="1"/>
+        <n v="137756" u="1"/>
         <n v="204" u="1"/>
         <n v="43124" u="1"/>
+        <n v="134428" u="1"/>
+        <n v="137268" u="1"/>
+        <n v="137836" u="1"/>
         <n v="6288" u="1"/>
         <n v="25896" u="1"/>
         <n v="73656" u="1"/>
+        <n v="137792" u="1"/>
         <n v="6648" u="1"/>
         <n v="5692" u="1"/>
         <n v="62252" u="1"/>
@@ -3718,6 +4060,7 @@
         <n v="61520" u="1"/>
         <n v="134172" u="1"/>
         <n v="134740" u="1"/>
+        <n v="137864" u="1"/>
         <n v="1372" u="1"/>
         <n v="17192" u="1"/>
         <n v="81684" u="1"/>
@@ -3740,15 +4083,22 @@
         <n v="58820" u="1"/>
         <n v="133312" u="1"/>
         <n v="136152" u="1"/>
+        <n v="137856" u="1"/>
         <n v="54012" u="1"/>
         <n v="68332" u="1"/>
         <n v="22100" u="1"/>
         <n v="51192" u="1"/>
+        <n v="73200" u="1"/>
         <n v="80584" u="1"/>
+        <n v="123752" u="1"/>
         <n v="52916" u="1"/>
+        <n v="136960" u="1"/>
         <n v="47540" u="1"/>
         <n v="48108" u="1"/>
+        <n v="65612" u="1"/>
         <n v="80664" u="1"/>
+        <n v="134768" u="1"/>
+        <n v="137608" u="1"/>
         <n v="13364" u="1"/>
         <n v="22992" u="1"/>
         <n v="35652" u="1"/>
@@ -3767,12 +4117,14 @@
         <n v="47720" u="1"/>
         <n v="79928" u="1"/>
         <n v="69744" u="1"/>
+        <n v="138204" u="1"/>
         <n v="53196" u="1"/>
         <n v="77532" u="1"/>
         <n v="134752" u="1"/>
         <n v="20708" u="1"/>
         <n v="47272" u="1"/>
         <n v="48408" u="1"/>
+        <n v="137388" u="1"/>
         <n v="40760" u="1"/>
         <n v="66576" u="1"/>
         <n v="134708" u="1"/>
@@ -3780,6 +4132,7 @@
         <n v="69212" u="1"/>
         <n v="71240" u="1"/>
         <n v="76352" u="1"/>
+        <n v="120656" u="1"/>
         <n v="134664" u="1"/>
         <n v="137788" u="1"/>
         <n v="50516" u="1"/>
@@ -3797,6 +4150,7 @@
         <n v="60516" u="1"/>
         <n v="93268" u="1"/>
         <n v="136120" u="1"/>
+        <n v="137824" u="1"/>
         <n v="22512" u="1"/>
         <n v="69736" u="1"/>
         <n v="78540" u="1"/>
@@ -3804,6 +4158,7 @@
         <n v="2800" u="1"/>
         <n v="56864" u="1"/>
         <n v="48080" u="1"/>
+        <n v="133520" u="1"/>
         <n v="2412" u="1"/>
         <n v="23536" u="1"/>
         <n v="30920" u="1"/>
@@ -3814,37 +4169,37 @@
         <n v="123572" u="1"/>
         <n v="46436" u="1"/>
         <n v="59520" u="1"/>
+        <n v="134976" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="THREADID" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="118496" maxValue="136700" count="6">
-        <n v="135128"/>
-        <n v="136568"/>
-        <n v="136700"/>
-        <n v="132888"/>
-        <n v="136312"/>
-        <n v="118496"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="54988" maxValue="138304" count="3">
+        <n v="54988"/>
+        <n v="138304"/>
+        <n v="137352" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="NETPROCESSID" numFmtId="0" sqlType="6">
-      <sharedItems containsString="0" containsBlank="1" count="1">
-        <m/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="133100" maxValue="139476" count="2">
+        <n v="133100"/>
+        <n v="139476"/>
       </sharedItems>
     </cacheField>
     <cacheField name="NETTHREADID" numFmtId="0" sqlType="6">
-      <sharedItems containsString="0" containsBlank="1" count="1">
-        <m/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="54988" maxValue="138304" count="2">
+        <n v="54988"/>
+        <n v="138304"/>
       </sharedItems>
     </cacheField>
     <cacheField name="POS" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="5939"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="539"/>
     </cacheField>
     <cacheField name="FEATUREID" numFmtId="0" sqlType="6">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="3" count="4">
+        <n v="0"/>
+        <n v="1"/>
         <n v="2"/>
         <n v="3"/>
-        <n v="0"/>
-        <n v="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="ACTUAL" numFmtId="0" sqlType="6">
@@ -3863,13 +4218,13 @@
       </sharedItems>
     </cacheField>
     <cacheField name="ACTUALTRS" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-1.00000023841858" maxValue="1"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-1" maxValue="1"/>
     </cacheField>
     <cacheField name="PREDICTEDTRS" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-0.77474886178970304" maxValue="0.77143287658691395"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-0.66471564769744895" maxValue="0.65950626134872403"/>
     </cacheField>
     <cacheField name="ERRORTRS" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2.12341547012329E-7" maxValue="1.2204825878143299"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.29342079162598E-5" maxValue="1.2624430656433101"/>
     </cacheField>
     <cacheField name="BARWIDTH" numFmtId="0" sqlType="6">
       <sharedItems containsString="0" containsBlank="1" count="1">
@@ -4867,179 +5222,207 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" fieldListSortAscending="1">
-  <location ref="A3:F11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="48" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" fieldListSortAscending="1">
+  <location ref="A3:D10" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="14">
-    <pivotField axis="axisRow" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="156">
+    <pivotField axis="axisCol" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
+      <items count="177">
+        <item m="1" x="5"/>
+        <item m="1" x="81"/>
+        <item m="1" x="166"/>
+        <item m="1" x="48"/>
+        <item m="1" x="118"/>
+        <item m="1" x="146"/>
+        <item m="1" x="69"/>
+        <item m="1" x="128"/>
+        <item m="1" x="93"/>
+        <item m="1" x="158"/>
+        <item m="1" x="82"/>
+        <item m="1" x="85"/>
+        <item m="1" x="167"/>
+        <item m="1" x="59"/>
+        <item m="1" x="144"/>
+        <item m="1" x="126"/>
+        <item m="1" x="83"/>
+        <item m="1" x="43"/>
+        <item m="1" x="68"/>
+        <item m="1" x="63"/>
+        <item m="1" x="39"/>
+        <item m="1" x="162"/>
+        <item m="1" x="53"/>
+        <item m="1" x="52"/>
+        <item m="1" x="6"/>
+        <item m="1" x="170"/>
+        <item m="1" x="106"/>
+        <item m="1" x="38"/>
+        <item m="1" x="22"/>
+        <item m="1" x="23"/>
+        <item m="1" x="72"/>
+        <item m="1" x="40"/>
+        <item m="1" x="107"/>
+        <item m="1" x="12"/>
+        <item m="1" x="152"/>
+        <item m="1" x="56"/>
+        <item m="1" x="49"/>
+        <item m="1" x="73"/>
+        <item m="1" x="117"/>
+        <item m="1" x="168"/>
+        <item m="1" x="135"/>
+        <item m="1" x="111"/>
+        <item m="1" x="33"/>
+        <item m="1" x="57"/>
+        <item m="1" x="108"/>
+        <item m="1" x="34"/>
+        <item m="1" x="7"/>
+        <item m="1" x="86"/>
+        <item m="1" x="15"/>
+        <item m="1" x="74"/>
+        <item m="1" x="169"/>
+        <item m="1" x="132"/>
+        <item m="1" x="75"/>
+        <item m="1" x="171"/>
+        <item m="1" x="76"/>
+        <item m="1" x="44"/>
+        <item m="1" x="153"/>
+        <item m="1" x="17"/>
+        <item m="1" x="24"/>
+        <item m="1" x="29"/>
+        <item m="1" x="13"/>
+        <item m="1" x="147"/>
+        <item m="1" x="58"/>
+        <item m="1" x="174"/>
+        <item m="1" x="35"/>
+        <item m="1" x="129"/>
+        <item m="1" x="41"/>
+        <item m="1" x="100"/>
+        <item m="1" x="113"/>
+        <item m="1" x="121"/>
+        <item m="1" x="164"/>
+        <item m="1" x="101"/>
+        <item m="1" x="109"/>
+        <item m="1" x="18"/>
+        <item m="1" x="130"/>
+        <item m="1" x="30"/>
+        <item m="1" x="148"/>
+        <item m="1" x="116"/>
+        <item m="1" x="142"/>
+        <item m="1" x="98"/>
+        <item m="1" x="125"/>
+        <item m="1" x="91"/>
+        <item m="1" x="25"/>
+        <item m="1" x="163"/>
+        <item m="1" x="3"/>
+        <item m="1" x="87"/>
+        <item m="1" x="27"/>
+        <item m="1" x="36"/>
+        <item m="1" x="175"/>
+        <item m="1" x="154"/>
+        <item m="1" x="64"/>
+        <item m="1" x="150"/>
+        <item m="1" x="54"/>
+        <item m="1" x="143"/>
+        <item m="1" x="133"/>
+        <item m="1" x="77"/>
+        <item m="1" x="92"/>
+        <item m="1" x="136"/>
+        <item m="1" x="159"/>
+        <item m="1" x="123"/>
+        <item m="1" x="137"/>
+        <item m="1" x="50"/>
+        <item m="1" x="78"/>
+        <item m="1" x="172"/>
+        <item m="1" x="138"/>
+        <item m="1" x="37"/>
+        <item m="1" x="151"/>
+        <item m="1" x="55"/>
+        <item m="1" x="160"/>
+        <item m="1" x="122"/>
+        <item m="1" x="96"/>
+        <item m="1" x="26"/>
+        <item m="1" x="103"/>
+        <item m="1" x="79"/>
+        <item m="1" x="70"/>
+        <item m="1" x="2"/>
+        <item m="1" x="19"/>
         <item m="1" x="8"/>
-        <item m="1" x="72"/>
+        <item m="1" x="80"/>
+        <item m="1" x="110"/>
+        <item m="1" x="62"/>
+        <item m="1" x="149"/>
+        <item m="1" x="9"/>
+        <item m="1" x="155"/>
         <item m="1" x="145"/>
-        <item m="1" x="41"/>
+        <item m="1" x="112"/>
+        <item m="1" x="88"/>
+        <item m="1" x="173"/>
+        <item m="1" x="134"/>
+        <item m="1" x="127"/>
+        <item m="1" x="32"/>
+        <item m="1" x="140"/>
+        <item m="1" x="71"/>
+        <item m="1" x="119"/>
+        <item m="1" x="114"/>
+        <item m="1" x="94"/>
+        <item m="1" x="89"/>
+        <item m="1" x="156"/>
+        <item m="1" x="61"/>
+        <item m="1" x="120"/>
+        <item m="1" x="141"/>
+        <item m="1" x="115"/>
+        <item m="1" x="60"/>
+        <item m="1" x="161"/>
+        <item m="1" x="16"/>
+        <item m="1" x="65"/>
+        <item m="1" x="66"/>
+        <item m="1" x="84"/>
+        <item m="1" x="31"/>
+        <item m="1" x="165"/>
+        <item m="1" x="176"/>
+        <item m="1" x="11"/>
+        <item m="1" x="99"/>
+        <item m="1" x="21"/>
+        <item m="1" x="90"/>
+        <item m="1" x="104"/>
+        <item m="1" x="10"/>
+        <item m="1" x="157"/>
+        <item m="1" x="47"/>
+        <item m="1" x="67"/>
+        <item m="1" x="20"/>
+        <item m="1" x="139"/>
+        <item m="1" x="4"/>
+        <item m="1" x="131"/>
+        <item m="1" x="42"/>
+        <item m="1" x="28"/>
+        <item m="1" x="14"/>
+        <item m="1" x="45"/>
         <item m="1" x="102"/>
-        <item m="1" x="127"/>
-        <item m="1" x="60"/>
-        <item m="1" x="111"/>
-        <item m="1" x="83"/>
-        <item m="1" x="138"/>
-        <item m="1" x="73"/>
-        <item m="1" x="76"/>
-        <item m="1" x="146"/>
+        <item m="1" x="95"/>
+        <item m="1" x="46"/>
+        <item m="1" x="105"/>
         <item m="1" x="51"/>
-        <item m="1" x="125"/>
-        <item m="1" x="109"/>
-        <item m="1" x="74"/>
-        <item m="1" x="39"/>
-        <item m="1" x="59"/>
-        <item m="1" x="55"/>
-        <item m="1" x="36"/>
-        <item m="1" x="142"/>
-        <item m="1" x="45"/>
-        <item m="1" x="44"/>
-        <item m="1" x="9"/>
-        <item m="1" x="149"/>
-        <item m="1" x="90"/>
-        <item m="1" x="35"/>
-        <item m="1" x="20"/>
-        <item m="1" x="21"/>
-        <item m="1" x="63"/>
-        <item m="1" x="37"/>
-        <item m="1" x="91"/>
-        <item m="1" x="13"/>
-        <item m="1" x="133"/>
-        <item m="1" x="48"/>
-        <item m="1" x="42"/>
-        <item m="1" x="64"/>
-        <item m="1" x="101"/>
-        <item m="1" x="147"/>
-        <item m="1" x="117"/>
-        <item m="1" x="95"/>
-        <item m="1" x="30"/>
-        <item m="1" x="49"/>
-        <item m="1" x="92"/>
-        <item m="1" x="31"/>
-        <item m="1" x="10"/>
-        <item m="1" x="77"/>
-        <item m="1" x="15"/>
-        <item m="1" x="65"/>
-        <item m="1" x="148"/>
-        <item m="1" x="114"/>
-        <item m="1" x="66"/>
-        <item m="1" x="150"/>
-        <item m="1" x="67"/>
-        <item m="1" x="40"/>
-        <item m="1" x="134"/>
-        <item m="1" x="17"/>
-        <item m="1" x="22"/>
-        <item m="1" x="26"/>
-        <item m="1" x="14"/>
-        <item m="1" x="128"/>
-        <item m="1" x="50"/>
-        <item m="1" x="153"/>
-        <item m="1" x="32"/>
-        <item m="1" x="112"/>
-        <item m="1" x="38"/>
-        <item m="1" x="87"/>
+        <item m="1" x="124"/>
         <item m="1" x="97"/>
-        <item m="1" x="105"/>
-        <item m="1" x="144"/>
-        <item m="1" x="88"/>
-        <item m="1" x="93"/>
-        <item m="1" x="18"/>
-        <item m="1" x="113"/>
-        <item m="1" x="27"/>
-        <item m="1" x="129"/>
-        <item m="1" x="100"/>
-        <item m="1" x="123"/>
-        <item m="1" x="86"/>
-        <item m="1" x="108"/>
-        <item m="1" x="81"/>
-        <item m="1" x="23"/>
-        <item m="1" x="143"/>
-        <item m="1" x="7"/>
-        <item m="1" x="78"/>
-        <item m="1" x="25"/>
-        <item m="1" x="33"/>
-        <item m="1" x="154"/>
-        <item m="1" x="135"/>
-        <item m="1" x="56"/>
-        <item m="1" x="131"/>
-        <item m="1" x="46"/>
-        <item m="1" x="124"/>
-        <item m="1" x="115"/>
-        <item m="1" x="68"/>
-        <item m="1" x="82"/>
-        <item m="1" x="118"/>
-        <item m="1" x="139"/>
-        <item m="1" x="107"/>
-        <item m="1" x="119"/>
-        <item m="1" x="43"/>
-        <item m="1" x="69"/>
-        <item m="1" x="151"/>
-        <item m="1" x="120"/>
-        <item m="1" x="34"/>
-        <item m="1" x="132"/>
-        <item m="1" x="47"/>
-        <item m="1" x="140"/>
-        <item m="1" x="106"/>
-        <item m="1" x="85"/>
-        <item m="1" x="24"/>
-        <item m="1" x="89"/>
-        <item m="1" x="70"/>
-        <item m="1" x="61"/>
-        <item m="1" x="6"/>
-        <item m="1" x="19"/>
-        <item m="1" x="11"/>
-        <item m="1" x="71"/>
-        <item m="1" x="94"/>
-        <item m="1" x="54"/>
-        <item m="1" x="130"/>
-        <item m="1" x="12"/>
-        <item m="1" x="136"/>
-        <item m="1" x="126"/>
-        <item m="1" x="96"/>
-        <item m="1" x="79"/>
-        <item m="1" x="152"/>
-        <item m="1" x="116"/>
-        <item m="1" x="110"/>
-        <item m="1" x="29"/>
-        <item m="1" x="121"/>
-        <item m="1" x="62"/>
-        <item m="1" x="103"/>
-        <item m="1" x="98"/>
-        <item m="1" x="84"/>
-        <item m="1" x="80"/>
-        <item m="1" x="137"/>
-        <item m="1" x="53"/>
-        <item m="1" x="104"/>
-        <item m="1" x="122"/>
-        <item m="1" x="99"/>
-        <item m="1" x="52"/>
-        <item m="1" x="141"/>
-        <item m="1" x="16"/>
-        <item m="1" x="57"/>
-        <item m="1" x="58"/>
-        <item m="1" x="75"/>
-        <item m="1" x="28"/>
         <item x="0"/>
         <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item m="1" x="2"/>
+        <item x="0"/>
+        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisRow" showAll="0">
       <items count="5">
+        <item x="0"/>
+        <item x="1"/>
         <item x="2"/>
         <item x="3"/>
-        <item x="0"/>
-        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -5053,35 +5436,9 @@
     <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="0"/>
+    <field x="5"/>
   </rowFields>
-  <rowItems count="7">
-    <i>
-      <x v="149"/>
-    </i>
-    <i>
-      <x v="150"/>
-    </i>
-    <i>
-      <x v="151"/>
-    </i>
-    <i>
-      <x v="152"/>
-    </i>
-    <i>
-      <x v="153"/>
-    </i>
-    <i>
-      <x v="154"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="5"/>
-  </colFields>
-  <colItems count="5">
+  <rowItems count="5">
     <i>
       <x/>
     </i>
@@ -5097,11 +5454,28 @@
     <i t="grand">
       <x/>
     </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="0"/>
+    <field x="1"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x v="175"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="176"/>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
   </colItems>
   <dataFields count="1">
     <dataField name="Average of ERRORTRS" fld="11" subtotal="average" baseField="4" baseItem="0" numFmtId="164"/>
   </dataFields>
-  <chartFormats count="5">
+  <chartFormats count="35">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -5155,6 +5529,435 @@
           </reference>
           <reference field="5" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="157"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="158"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="151"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="152"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="154"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="155"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="11" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="157"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="12" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="158"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="13" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="159"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="14" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="149"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="15" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="150"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="16" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="154"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="17" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="155"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="18" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="156"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="19" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="158"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="20" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="159"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="21" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="149"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="22" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="152"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="23" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="153"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="24" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="155"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="25" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="156"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="26" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="157"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="27" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="159"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="28" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="166"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="29" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="168"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="30" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="169"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="31" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="170"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="32" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="171"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="33" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="172"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="34" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="173"/>
           </reference>
         </references>
       </pivotArea>
@@ -5384,162 +6187,184 @@
   </pivotTables>
   <data>
     <tabular pivotCacheId="2">
-      <items count="155">
+      <items count="177">
         <i x="0" s="1"/>
         <i x="1" s="1"/>
-        <i x="2" s="1"/>
-        <i x="3" s="1"/>
-        <i x="4" s="1"/>
-        <i x="5" s="1"/>
+        <i x="43" s="1" nd="1"/>
+        <i x="68" s="1" nd="1"/>
+        <i x="63" s="1" nd="1"/>
+        <i x="5" s="1" nd="1"/>
+        <i x="81" s="1" nd="1"/>
+        <i x="166" s="1" nd="1"/>
         <i x="39" s="1" nd="1"/>
+        <i x="162" s="1" nd="1"/>
+        <i x="53" s="1" nd="1"/>
+        <i x="48" s="1" nd="1"/>
+        <i x="52" s="1" nd="1"/>
+        <i x="118" s="1" nd="1"/>
+        <i x="146" s="1" nd="1"/>
+        <i x="6" s="1" nd="1"/>
+        <i x="170" s="1" nd="1"/>
+        <i x="106" s="1" nd="1"/>
+        <i x="38" s="1" nd="1"/>
+        <i x="22" s="1" nd="1"/>
+        <i x="69" s="1" nd="1"/>
+        <i x="23" s="1" nd="1"/>
+        <i x="72" s="1" nd="1"/>
+        <i x="128" s="1" nd="1"/>
+        <i x="40" s="1" nd="1"/>
+        <i x="93" s="1" nd="1"/>
+        <i x="158" s="1" nd="1"/>
+        <i x="82" s="1" nd="1"/>
+        <i x="107" s="1" nd="1"/>
+        <i x="85" s="1" nd="1"/>
+        <i x="167" s="1" nd="1"/>
+        <i x="12" s="1" nd="1"/>
+        <i x="152" s="1" nd="1"/>
+        <i x="32" s="1" nd="1"/>
+        <i x="56" s="1" nd="1"/>
+        <i x="49" s="1" nd="1"/>
+        <i x="73" s="1" nd="1"/>
+        <i x="117" s="1" nd="1"/>
+        <i x="168" s="1" nd="1"/>
+        <i x="135" s="1" nd="1"/>
+        <i x="111" s="1" nd="1"/>
+        <i x="33" s="1" nd="1"/>
+        <i x="57" s="1" nd="1"/>
+        <i x="108" s="1" nd="1"/>
+        <i x="34" s="1" nd="1"/>
+        <i x="7" s="1" nd="1"/>
+        <i x="86" s="1" nd="1"/>
+        <i x="20" s="1" nd="1"/>
+        <i x="15" s="1" nd="1"/>
+        <i x="74" s="1" nd="1"/>
+        <i x="169" s="1" nd="1"/>
+        <i x="132" s="1" nd="1"/>
+        <i x="75" s="1" nd="1"/>
+        <i x="171" s="1" nd="1"/>
+        <i x="76" s="1" nd="1"/>
+        <i x="44" s="1" nd="1"/>
+        <i x="153" s="1" nd="1"/>
+        <i x="17" s="1" nd="1"/>
+        <i x="24" s="1" nd="1"/>
+        <i x="29" s="1" nd="1"/>
+        <i x="13" s="1" nd="1"/>
+        <i x="147" s="1" nd="1"/>
+        <i x="58" s="1" nd="1"/>
+        <i x="174" s="1" nd="1"/>
+        <i x="35" s="1" nd="1"/>
+        <i x="129" s="1" nd="1"/>
+        <i x="41" s="1" nd="1"/>
+        <i x="100" s="1" nd="1"/>
+        <i x="113" s="1" nd="1"/>
+        <i x="121" s="1" nd="1"/>
+        <i x="164" s="1" nd="1"/>
+        <i x="101" s="1" nd="1"/>
+        <i x="109" s="1" nd="1"/>
+        <i x="18" s="1" nd="1"/>
+        <i x="130" s="1" nd="1"/>
+        <i x="30" s="1" nd="1"/>
+        <i x="148" s="1" nd="1"/>
+        <i x="116" s="1" nd="1"/>
+        <i x="142" s="1" nd="1"/>
+        <i x="94" s="1" nd="1"/>
+        <i x="98" s="1" nd="1"/>
+        <i x="125" s="1" nd="1"/>
+        <i x="91" s="1" nd="1"/>
+        <i x="25" s="1" nd="1"/>
+        <i x="163" s="1" nd="1"/>
+        <i x="3" s="1" nd="1"/>
+        <i x="87" s="1" nd="1"/>
+        <i x="27" s="1" nd="1"/>
         <i x="59" s="1" nd="1"/>
+        <i x="36" s="1" nd="1"/>
+        <i x="175" s="1" nd="1"/>
+        <i x="154" s="1" nd="1"/>
+        <i x="64" s="1" nd="1"/>
+        <i x="150" s="1" nd="1"/>
+        <i x="54" s="1" nd="1"/>
+        <i x="143" s="1" nd="1"/>
+        <i x="102" s="1" nd="1"/>
+        <i x="133" s="1" nd="1"/>
+        <i x="77" s="1" nd="1"/>
+        <i x="92" s="1" nd="1"/>
+        <i x="136" s="1" nd="1"/>
+        <i x="159" s="1" nd="1"/>
+        <i x="123" s="1" nd="1"/>
+        <i x="137" s="1" nd="1"/>
+        <i x="95" s="1" nd="1"/>
+        <i x="50" s="1" nd="1"/>
+        <i x="78" s="1" nd="1"/>
+        <i x="172" s="1" nd="1"/>
+        <i x="138" s="1" nd="1"/>
+        <i x="37" s="1" nd="1"/>
+        <i x="144" s="1" nd="1"/>
+        <i x="126" s="1" nd="1"/>
+        <i x="151" s="1" nd="1"/>
+        <i x="83" s="1" nd="1"/>
         <i x="55" s="1" nd="1"/>
+        <i x="160" s="1" nd="1"/>
+        <i x="122" s="1" nd="1"/>
+        <i x="96" s="1" nd="1"/>
+        <i x="26" s="1" nd="1"/>
+        <i x="103" s="1" nd="1"/>
+        <i x="79" s="1" nd="1"/>
+        <i x="70" s="1" nd="1"/>
+        <i x="2" s="1" nd="1"/>
+        <i x="19" s="1" nd="1"/>
         <i x="8" s="1" nd="1"/>
-        <i x="72" s="1" nd="1"/>
-        <i x="145" s="1" nd="1"/>
-        <i x="36" s="1" nd="1"/>
-        <i x="142" s="1" nd="1"/>
-        <i x="45" s="1" nd="1"/>
-        <i x="41" s="1" nd="1"/>
-        <i x="44" s="1" nd="1"/>
-        <i x="102" s="1" nd="1"/>
-        <i x="127" s="1" nd="1"/>
-        <i x="9" s="1" nd="1"/>
-        <i x="149" s="1" nd="1"/>
-        <i x="90" s="1" nd="1"/>
-        <i x="35" s="1" nd="1"/>
-        <i x="20" s="1" nd="1"/>
-        <i x="60" s="1" nd="1"/>
-        <i x="21" s="1" nd="1"/>
-        <i x="63" s="1" nd="1"/>
-        <i x="111" s="1" nd="1"/>
-        <i x="37" s="1" nd="1"/>
-        <i x="83" s="1" nd="1"/>
-        <i x="138" s="1" nd="1"/>
-        <i x="73" s="1" nd="1"/>
-        <i x="91" s="1" nd="1"/>
-        <i x="76" s="1" nd="1"/>
-        <i x="146" s="1" nd="1"/>
-        <i x="13" s="1" nd="1"/>
-        <i x="133" s="1" nd="1"/>
-        <i x="29" s="1" nd="1"/>
-        <i x="48" s="1" nd="1"/>
-        <i x="42" s="1" nd="1"/>
-        <i x="64" s="1" nd="1"/>
-        <i x="101" s="1" nd="1"/>
-        <i x="147" s="1" nd="1"/>
-        <i x="117" s="1" nd="1"/>
-        <i x="95" s="1" nd="1"/>
-        <i x="30" s="1" nd="1"/>
-        <i x="49" s="1" nd="1"/>
-        <i x="92" s="1" nd="1"/>
-        <i x="31" s="1" nd="1"/>
-        <i x="10" s="1" nd="1"/>
-        <i x="77" s="1" nd="1"/>
-        <i x="15" s="1" nd="1"/>
-        <i x="65" s="1" nd="1"/>
-        <i x="148" s="1" nd="1"/>
-        <i x="114" s="1" nd="1"/>
-        <i x="66" s="1" nd="1"/>
-        <i x="150" s="1" nd="1"/>
-        <i x="67" s="1" nd="1"/>
-        <i x="40" s="1" nd="1"/>
-        <i x="134" s="1" nd="1"/>
-        <i x="17" s="1" nd="1"/>
-        <i x="22" s="1" nd="1"/>
-        <i x="26" s="1" nd="1"/>
-        <i x="14" s="1" nd="1"/>
-        <i x="128" s="1" nd="1"/>
-        <i x="50" s="1" nd="1"/>
-        <i x="153" s="1" nd="1"/>
-        <i x="32" s="1" nd="1"/>
-        <i x="112" s="1" nd="1"/>
-        <i x="38" s="1" nd="1"/>
-        <i x="87" s="1" nd="1"/>
-        <i x="97" s="1" nd="1"/>
-        <i x="105" s="1" nd="1"/>
-        <i x="144" s="1" nd="1"/>
-        <i x="88" s="1" nd="1"/>
-        <i x="93" s="1" nd="1"/>
-        <i x="18" s="1" nd="1"/>
-        <i x="113" s="1" nd="1"/>
-        <i x="27" s="1" nd="1"/>
-        <i x="129" s="1" nd="1"/>
-        <i x="100" s="1" nd="1"/>
-        <i x="123" s="1" nd="1"/>
-        <i x="84" s="1" nd="1"/>
-        <i x="86" s="1" nd="1"/>
-        <i x="108" s="1" nd="1"/>
-        <i x="81" s="1" nd="1"/>
-        <i x="23" s="1" nd="1"/>
-        <i x="143" s="1" nd="1"/>
-        <i x="7" s="1" nd="1"/>
-        <i x="78" s="1" nd="1"/>
-        <i x="25" s="1" nd="1"/>
-        <i x="51" s="1" nd="1"/>
-        <i x="33" s="1" nd="1"/>
-        <i x="154" s="1" nd="1"/>
-        <i x="135" s="1" nd="1"/>
-        <i x="56" s="1" nd="1"/>
-        <i x="131" s="1" nd="1"/>
-        <i x="46" s="1" nd="1"/>
-        <i x="124" s="1" nd="1"/>
-        <i x="115" s="1" nd="1"/>
-        <i x="68" s="1" nd="1"/>
-        <i x="82" s="1" nd="1"/>
-        <i x="118" s="1" nd="1"/>
-        <i x="139" s="1" nd="1"/>
-        <i x="107" s="1" nd="1"/>
-        <i x="119" s="1" nd="1"/>
-        <i x="43" s="1" nd="1"/>
-        <i x="69" s="1" nd="1"/>
-        <i x="151" s="1" nd="1"/>
-        <i x="120" s="1" nd="1"/>
-        <i x="34" s="1" nd="1"/>
-        <i x="125" s="1" nd="1"/>
-        <i x="109" s="1" nd="1"/>
-        <i x="132" s="1" nd="1"/>
-        <i x="74" s="1" nd="1"/>
-        <i x="47" s="1" nd="1"/>
-        <i x="140" s="1" nd="1"/>
-        <i x="106" s="1" nd="1"/>
-        <i x="85" s="1" nd="1"/>
-        <i x="24" s="1" nd="1"/>
-        <i x="89" s="1" nd="1"/>
-        <i x="70" s="1" nd="1"/>
-        <i x="61" s="1" nd="1"/>
-        <i x="6" s="1" nd="1"/>
-        <i x="19" s="1" nd="1"/>
-        <i x="11" s="1" nd="1"/>
-        <i x="71" s="1" nd="1"/>
-        <i x="94" s="1" nd="1"/>
-        <i x="54" s="1" nd="1"/>
-        <i x="130" s="1" nd="1"/>
-        <i x="141" s="1" nd="1"/>
-        <i x="12" s="1" nd="1"/>
-        <i x="136" s="1" nd="1"/>
-        <i x="126" s="1" nd="1"/>
-        <i x="103" s="1" nd="1"/>
-        <i x="96" s="1" nd="1"/>
-        <i x="152" s="1" nd="1"/>
-        <i x="79" s="1" nd="1"/>
-        <i x="98" s="1" nd="1"/>
-        <i x="52" s="1" nd="1"/>
-        <i x="16" s="1" nd="1"/>
-        <i x="57" s="1" nd="1"/>
-        <i x="121" s="1" nd="1"/>
-        <i x="116" s="1" nd="1"/>
-        <i x="58" s="1" nd="1"/>
+        <i x="80" s="1" nd="1"/>
         <i x="110" s="1" nd="1"/>
         <i x="62" s="1" nd="1"/>
-        <i x="75" s="1" nd="1"/>
-        <i x="137" s="1" nd="1"/>
-        <i x="80" s="1" nd="1"/>
-        <i x="53" s="1" nd="1"/>
+        <i x="149" s="1" nd="1"/>
+        <i x="161" s="1" nd="1"/>
+        <i x="9" s="1" nd="1"/>
+        <i x="155" s="1" nd="1"/>
+        <i x="145" s="1" nd="1"/>
+        <i x="119" s="1" nd="1"/>
+        <i x="112" s="1" nd="1"/>
+        <i x="139" s="1" nd="1"/>
+        <i x="173" s="1" nd="1"/>
+        <i x="97" s="1" nd="1"/>
+        <i x="88" s="1" nd="1"/>
+        <i x="114" s="1" nd="1"/>
+        <i x="165" s="1" nd="1"/>
+        <i x="60" s="1" nd="1"/>
+        <i x="16" s="1" nd="1"/>
+        <i x="65" s="1" nd="1"/>
+        <i x="14" s="1" nd="1"/>
+        <i x="45" s="1" nd="1"/>
+        <i x="140" s="1" nd="1"/>
+        <i x="134" s="1" nd="1"/>
+        <i x="66" s="1" nd="1"/>
+        <i x="127" s="1" nd="1"/>
+        <i x="104" s="1" nd="1"/>
+        <i x="71" s="1" nd="1"/>
+        <i x="4" s="1" nd="1"/>
+        <i x="176" s="1" nd="1"/>
+        <i x="84" s="1" nd="1"/>
+        <i x="11" s="1" nd="1"/>
+        <i x="156" s="1" nd="1"/>
+        <i x="89" s="1" nd="1"/>
+        <i x="61" s="1" nd="1"/>
+        <i x="99" s="1" nd="1"/>
+        <i x="10" s="1" nd="1"/>
+        <i x="31" s="1" nd="1"/>
+        <i x="21" s="1" nd="1"/>
+        <i x="46" s="1" nd="1"/>
+        <i x="131" s="1" nd="1"/>
+        <i x="105" s="1" nd="1"/>
+        <i x="120" s="1" nd="1"/>
+        <i x="42" s="1" nd="1"/>
+        <i x="141" s="1" nd="1"/>
+        <i x="51" s="1" nd="1"/>
+        <i x="157" s="1" nd="1"/>
+        <i x="47" s="1" nd="1"/>
+        <i x="90" s="1" nd="1"/>
+        <i x="67" s="1" nd="1"/>
+        <i x="124" s="1" nd="1"/>
         <i x="28" s="1" nd="1"/>
-        <i x="104" s="1" nd="1"/>
-        <i x="122" s="1" nd="1"/>
-        <i x="99" s="1" nd="1"/>
+        <i x="115" s="1" nd="1"/>
       </items>
     </tabular>
   </data>
@@ -7029,23 +7854,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F11"/>
+  <dimension ref="A3:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="8" width="7.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="12" width="7.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" customWidth="1"/>
+    <col min="14" max="32" width="7.5703125" customWidth="1"/>
+    <col min="33" max="33" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -7053,140 +7882,96 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
-      </c>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4">
+        <v>133100</v>
+      </c>
+      <c r="C4">
+        <v>139476</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>54988</v>
+      </c>
+      <c r="C5">
+        <v>138304</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
+      <c r="B6" s="1">
+        <v>4.0951737113021039E-2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4.0951737113021039E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4.0951737113021039E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>5.6764620197591958E-2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5.6764620197591958E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5.6764620197591958E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>2</v>
       </c>
-      <c r="E4">
+      <c r="B8" s="1">
+        <v>7.1587257583936068E-2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7.1587257583936068E-2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>7.1587257583936068E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="B9" s="1">
+        <v>8.2925817798133253E-2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8.2925817798133253E-2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>8.2925817798133253E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>133520</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1">
-        <v>3.9946007234232909E-2</v>
-      </c>
-      <c r="E5" s="1">
-        <v>4.2206446785065861E-2</v>
-      </c>
-      <c r="F5" s="1">
-        <v>4.1076227009649385E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>134976</v>
-      </c>
-      <c r="B6" s="1">
-        <v>3.3141288456666952E-2</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1">
-        <v>4.5915680880554852E-2</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1">
-        <v>3.9528484668610898E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>136024</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3.515897625147895E-2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>3.883773612943462E-2</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1">
-        <v>3.6998356190456785E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>136960</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1">
-        <v>3.3955207038106339E-2</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1">
-        <v>4.2783293378874911E-2</v>
-      </c>
-      <c r="F8" s="1">
-        <v>3.8369250208490628E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>137196</v>
-      </c>
-      <c r="B9" s="1">
-        <v>5.0300426752955627E-3</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1">
-        <v>4.2798512137999838E-2</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2.3914277406647703E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>137856</v>
-      </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1">
+        <v>6.3057358173170569E-2</v>
+      </c>
       <c r="C10" s="1">
-        <v>3.7888838628288173E-2</v>
+        <v>6.3057358173170569E-2</v>
       </c>
       <c r="D10" s="1">
-        <v>4.5688435739856405E-2</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1">
-        <v>4.1788637184072289E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1">
-        <v>2.4443435794480488E-2</v>
-      </c>
-      <c r="C11" s="1">
-        <v>3.6893927265276377E-2</v>
-      </c>
-      <c r="D11" s="1">
-        <v>4.3850041284881389E-2</v>
-      </c>
-      <c r="E11" s="1">
-        <v>4.2596084100646872E-2</v>
-      </c>
-      <c r="F11" s="1">
-        <v>3.6945872111321283E-2</v>
+        <v>6.3057358173170569E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some large-scale tests. not too happy...
</commit_message>
<xml_diff>
--- a/Tester2.xlsx
+++ b/Tester2.xlsx
@@ -25,8 +25,8 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="53" r:id="rId4"/>
-    <pivotCache cacheId="57" r:id="rId5"/>
+    <pivotCache cacheId="60" r:id="rId4"/>
+    <pivotCache cacheId="64" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -502,154 +502,154 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>2.9612287878990201E-2</c:v>
+                  <c:v>4.0237335488200196E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.06098556518555E-2</c:v>
+                  <c:v>3.8368329405784598E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9641065970063199E-2</c:v>
+                  <c:v>3.6540711298584899E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8915496766567199E-2</c:v>
+                  <c:v>3.5157108213752499E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.8520979210734399E-2</c:v>
+                  <c:v>3.47778992727399E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.8202744424343099E-2</c:v>
+                  <c:v>3.41971893794835E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.7816403880715401E-2</c:v>
+                  <c:v>3.3973550889640999E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.7425937578082099E-2</c:v>
+                  <c:v>3.3917247783392698E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.71273350715637E-2</c:v>
+                  <c:v>3.38736246339977E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.69132873415947E-2</c:v>
+                  <c:v>3.3852637279778702E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.6745075583457902E-2</c:v>
+                  <c:v>3.3826122526079399E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.65931023657322E-2</c:v>
+                  <c:v>3.3818443771451699E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.6450785100460101E-2</c:v>
+                  <c:v>3.37810162454844E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.6305642202496501E-2</c:v>
+                  <c:v>3.3748645801097198E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.6170406714081799E-2</c:v>
+                  <c:v>3.3637979067861999E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.6063641756772998E-2</c:v>
+                  <c:v>3.3517221454531002E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.5996532514691401E-2</c:v>
+                  <c:v>3.3405574504286099E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.5957765281200399E-2</c:v>
+                  <c:v>3.3347005955874898E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.5917852520942698E-2</c:v>
+                  <c:v>3.3300472423434301E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.58628057688475E-2</c:v>
+                  <c:v>3.3225200604647398E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.5785096213221501E-2</c:v>
+                  <c:v>3.3151437528431398E-3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.5681013464927701E-2</c:v>
+                  <c:v>3.3030060585588199E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.5545685775577999E-2</c:v>
+                  <c:v>3.2958749216049901E-3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.53756905347109E-2</c:v>
+                  <c:v>3.2886802218854401E-3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.5178616158664201E-2</c:v>
+                  <c:v>3.2848871778696801E-3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.49705493822694E-2</c:v>
+                  <c:v>3.2821216154843599E-3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.47744789719582E-2</c:v>
+                  <c:v>3.2788882963359399E-3</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.4620117843151099E-2</c:v>
+                  <c:v>3.2762323971837798E-3</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.4512683264911201E-2</c:v>
+                  <c:v>3.274105489254E-3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.44273331388831E-2</c:v>
+                  <c:v>3.2715781126171398E-3</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.4341021887957999E-2</c:v>
+                  <c:v>3.26960743404925E-3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.4250415377318901E-2</c:v>
+                  <c:v>3.2677173148840701E-3</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.41776716336608E-2</c:v>
+                  <c:v>3.26554221101105E-3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.41749801114202E-2</c:v>
+                  <c:v>3.2639687415212401E-3</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.42765445634723E-2</c:v>
+                  <c:v>3.2621894497424399E-3</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.4380438253283501E-2</c:v>
+                  <c:v>3.26066999696195E-3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.44595960155129E-2</c:v>
+                  <c:v>3.2594476360827702E-3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.4564007520675701E-2</c:v>
+                  <c:v>3.2581689301878201E-3</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.46931242197752E-2</c:v>
+                  <c:v>3.25711793266237E-3</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.4799563214182901E-2</c:v>
+                  <c:v>3.2561104744672801E-3</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.48293748497963E-2</c:v>
+                  <c:v>3.2551663462072598E-3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.4769732952117901E-2</c:v>
+                  <c:v>3.2543020788580201E-3</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1.4639918692409999E-2</c:v>
+                  <c:v>3.2534652855247298E-3</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.4463507570326301E-2</c:v>
+                  <c:v>3.2527185976505301E-3</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.4290274120867299E-2</c:v>
+                  <c:v>3.2519982196390598E-3</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.41516253352165E-2</c:v>
+                  <c:v>3.2513260375708298E-3</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.4036305248737301E-2</c:v>
+                  <c:v>3.2507032155990601E-3</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.39519507065415E-2</c:v>
+                  <c:v>3.2501004170626402E-3</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.39120882377028E-2</c:v>
+                  <c:v>3.24953813105822E-3</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.31871588528156E-2</c:v>
+                  <c:v>3.59822763130069E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1606,16 +1606,16 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4.1928980195963819E-2</c:v>
+                  <c:v>0.2772221380361804</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0340686032065639E-2</c:v>
+                  <c:v>0.51226119048617502</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0982940263218349E-2</c:v>
+                  <c:v>0.33369284981378805</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.9162700101733194E-2</c:v>
+                  <c:v>0.10929455532243956</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3185,7 +3185,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
@@ -3252,194 +3252,196 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="gcaglion" refreshedDate="43157.031755439813" createdVersion="6" refreshedVersion="5" minRefreshableVersion="3" recordCount="50">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="gcaglion" refreshedDate="43157.037984722221" createdVersion="6" refreshedVersion="5" minRefreshableVersion="3" recordCount="100">
   <cacheSource type="external" connectionId="2"/>
   <cacheFields count="5">
     <cacheField name="PROCESSID" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="204" maxValue="134028" count="178">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="204" maxValue="140220" count="179">
         <n v="43024"/>
+        <n v="140220"/>
+        <n v="42216" u="1"/>
+        <n v="82796" u="1"/>
+        <n v="57572" u="1"/>
+        <n v="1932" u="1"/>
+        <n v="7100" u="1"/>
+        <n v="36028" u="1"/>
+        <n v="78088" u="1"/>
+        <n v="84052" u="1"/>
+        <n v="92856" u="1"/>
+        <n v="49112" u="1"/>
+        <n v="120768" u="1"/>
+        <n v="24204" u="1"/>
+        <n v="30736" u="1"/>
+        <n v="44892" u="1"/>
+        <n v="59944" u="1"/>
+        <n v="39232" u="1"/>
+        <n v="43512" u="1"/>
+        <n v="48340" u="1"/>
+        <n v="83400" u="1"/>
+        <n v="16120" u="1"/>
+        <n v="15344" u="1"/>
+        <n v="18280" u="1"/>
+        <n v="43552" u="1"/>
+        <n v="54912" u="1"/>
+        <n v="80640" u="1"/>
+        <n v="58908" u="1"/>
+        <n v="44444" u="1"/>
+        <n v="48420" u="1"/>
+        <n v="134028" u="1"/>
+        <n v="32652" u="1"/>
+        <n v="35660" u="1"/>
+        <n v="46736" u="1"/>
+        <n v="59232" u="1"/>
+        <n v="75364" u="1"/>
+        <n v="76784" u="1"/>
+        <n v="15080" u="1"/>
+        <n v="90740" u="1"/>
+        <n v="2792" u="1"/>
+        <n v="21748" u="1"/>
+        <n v="47364" u="1"/>
+        <n v="204" u="1"/>
+        <n v="43124" u="1"/>
+        <n v="6288" u="1"/>
+        <n v="25896" u="1"/>
+        <n v="119624" u="1"/>
+        <n v="73656" u="1"/>
+        <n v="133248" u="1"/>
+        <n v="6648" u="1"/>
+        <n v="5692" u="1"/>
+        <n v="62252" u="1"/>
+        <n v="78280" u="1"/>
+        <n v="25652" u="1"/>
+        <n v="33304" u="1"/>
+        <n v="45516" u="1"/>
+        <n v="98200" u="1"/>
+        <n v="48964" u="1"/>
+        <n v="59188" u="1"/>
+        <n v="133364" u="1"/>
+        <n v="87852" u="1"/>
+        <n v="1540" u="1"/>
+        <n v="61520" u="1"/>
+        <n v="80792" u="1"/>
+        <n v="1372" u="1"/>
+        <n v="17192" u="1"/>
+        <n v="81684" u="1"/>
+        <n v="20184" u="1"/>
+        <n v="26432" u="1"/>
+        <n v="39408" u="1"/>
+        <n v="41964" u="1"/>
         <n v="77464" u="1"/>
+        <n v="133844" u="1"/>
+        <n v="42856" u="1"/>
+        <n v="68172" u="1"/>
+        <n v="75272" u="1"/>
+        <n v="81520" u="1"/>
+        <n v="84076" u="1"/>
+        <n v="2192" u="1"/>
+        <n v="5400" u="1"/>
+        <n v="22628" u="1"/>
+        <n v="71336" u="1"/>
+        <n v="78152" u="1"/>
+        <n v="33240" u="1"/>
+        <n v="133516" u="1"/>
+        <n v="23216" u="1"/>
         <n v="36100" u="1"/>
-        <n v="78280" u="1"/>
-        <n v="26432" u="1"/>
-        <n v="2412" u="1"/>
+        <n v="58820" u="1"/>
+        <n v="97828" u="1"/>
+        <n v="54012" u="1"/>
+        <n v="68332" u="1"/>
+        <n v="76000" u="1"/>
+        <n v="22100" u="1"/>
+        <n v="78028" u="1"/>
+        <n v="80584" u="1"/>
+        <n v="52916" u="1"/>
+        <n v="76648" u="1"/>
+        <n v="41008" u="1"/>
+        <n v="47540" u="1"/>
+        <n v="48108" u="1"/>
+        <n v="78960" u="1"/>
+        <n v="80664" u="1"/>
+        <n v="13364" u="1"/>
+        <n v="22992" u="1"/>
+        <n v="35652" u="1"/>
+        <n v="48148" u="1"/>
+        <n v="84436" u="1"/>
+        <n v="32516" u="1"/>
+        <n v="96972" u="1"/>
+        <n v="47620" u="1"/>
+        <n v="81108" u="1"/>
+        <n v="120584" u="1"/>
+        <n v="50480" u="1"/>
+        <n v="90804" u="1"/>
+        <n v="28712" u="1"/>
+        <n v="96524" u="1"/>
+        <n v="6888" u="1"/>
+        <n v="123828" u="1"/>
+        <n v="47720" u="1"/>
+        <n v="79928" u="1"/>
+        <n v="69744" u="1"/>
+        <n v="91368" u="1"/>
+        <n v="53196" u="1"/>
+        <n v="77776" u="1"/>
+        <n v="77532" u="1"/>
+        <n v="20708" u="1"/>
+        <n v="47272" u="1"/>
+        <n v="48408" u="1"/>
+        <n v="78992" u="1"/>
+        <n v="40760" u="1"/>
+        <n v="66576" u="1"/>
+        <n v="86740" u="1"/>
+        <n v="96112" u="1"/>
+        <n v="31956" u="1"/>
+        <n v="69212" u="1"/>
+        <n v="133164" u="1"/>
         <n v="71240" u="1"/>
-        <n v="81684" u="1"/>
+        <n v="76352" u="1"/>
+        <n v="50516" u="1"/>
+        <n v="65600" u="1"/>
+        <n v="77244" u="1"/>
+        <n v="94568" u="1"/>
+        <n v="7032" u="1"/>
+        <n v="21772" u="1"/>
+        <n v="45140" u="1"/>
         <n v="49400" u="1"/>
-        <n v="2192" u="1"/>
-        <n v="69212" u="1"/>
-        <n v="25896" u="1"/>
-        <n v="15344" u="1"/>
-        <n v="30920" u="1"/>
-        <n v="41008" u="1"/>
-        <n v="6648" u="1"/>
-        <n v="84436" u="1"/>
-        <n v="41964" u="1"/>
-        <n v="48340" u="1"/>
-        <n v="65600" u="1"/>
-        <n v="23536" u="1"/>
-        <n v="57572" u="1"/>
-        <n v="33304" u="1"/>
+        <n v="80976" u="1"/>
+        <n v="89780" u="1"/>
         <n v="98868" u="1"/>
-        <n v="71336" u="1"/>
+        <n v="52544" u="1"/>
         <n v="62200" u="1"/>
-        <n v="78540" u="1"/>
-        <n v="25652" u="1"/>
-        <n v="58820" u="1"/>
-        <n v="78960" u="1"/>
-        <n v="48108" u="1"/>
-        <n v="78028" u="1"/>
-        <n v="75860" u="1"/>
-        <n v="23216" u="1"/>
-        <n v="76000" u="1"/>
-        <n v="133248" u="1"/>
-        <n v="28712" u="1"/>
-        <n v="59520" u="1"/>
-        <n v="90804" u="1"/>
-        <n v="80640" u="1"/>
-        <n v="32652" u="1"/>
-        <n v="92856" u="1"/>
-        <n v="35660" u="1"/>
-        <n v="80664" u="1"/>
-        <n v="18280" u="1"/>
-        <n v="44892" u="1"/>
-        <n v="68332" u="1"/>
-        <n v="7100" u="1"/>
-        <n v="85840" u="1"/>
-        <n v="76352" u="1"/>
-        <n v="89780" u="1"/>
-        <n v="22628" u="1"/>
-        <n v="76632" u="1"/>
-        <n v="81108" u="1"/>
-        <n v="47620" u="1"/>
-        <n v="49112" u="1"/>
-        <n v="21748" u="1"/>
-        <n v="43552" u="1"/>
-        <n v="34204" u="1"/>
-        <n v="47364" u="1"/>
-        <n v="16120" u="1"/>
         <n v="77892" u="1"/>
-        <n v="56864" u="1"/>
-        <n v="77776" u="1"/>
-        <n v="22512" u="1"/>
-        <n v="133164" u="1"/>
-        <n v="68172" u="1"/>
-        <n v="91368" u="1"/>
         <n v="24348" u="1"/>
         <n v="43192" u="1"/>
-        <n v="21772" u="1"/>
-        <n v="47540" u="1"/>
-        <n v="47272" u="1"/>
-        <n v="15080" u="1"/>
-        <n v="119624" u="1"/>
-        <n v="46736" u="1"/>
-        <n v="90740" u="1"/>
-        <n v="98200" u="1"/>
-        <n v="30736" u="1"/>
+        <n v="45748" u="1"/>
+        <n v="60516" u="1"/>
+        <n v="83896" u="1"/>
+        <n v="93268" u="1"/>
+        <n v="22512" u="1"/>
         <n v="69736" u="1"/>
+        <n v="78540" u="1"/>
+        <n v="2800" u="1"/>
+        <n v="56864" u="1"/>
+        <n v="87384" u="1"/>
         <n v="134008" u="1"/>
-        <n v="78152" u="1"/>
-        <n v="59232" u="1"/>
-        <n v="87384" u="1"/>
-        <n v="97828" u="1"/>
-        <n v="5400" u="1"/>
-        <n v="1372" u="1"/>
-        <n v="78992" u="1"/>
-        <n v="120768" u="1"/>
+        <n v="48080" u="1"/>
+        <n v="76632" u="1"/>
+        <n v="2412" u="1"/>
+        <n v="23536" u="1"/>
+        <n v="30920" u="1"/>
+        <n v="39864" u="1"/>
+        <n v="11232" u="1"/>
+        <n v="34204" u="1"/>
         <n v="42156" u="1"/>
-        <n v="45140" u="1"/>
-        <n v="77244" u="1"/>
-        <n v="35652" u="1"/>
-        <n v="96524" u="1"/>
-        <n v="17192" u="1"/>
-        <n v="84052" u="1"/>
-        <n v="13364" u="1"/>
-        <n v="43124" u="1"/>
-        <n v="87852" u="1"/>
-        <n v="2800" u="1"/>
-        <n v="59944" u="1"/>
-        <n v="42856" u="1"/>
-        <n v="62252" u="1"/>
-        <n v="48148" u="1"/>
-        <n v="7032" u="1"/>
-        <n v="48964" u="1"/>
-        <n v="2792" u="1"/>
-        <n v="84076" u="1"/>
-        <n v="83400" u="1"/>
-        <n v="33240" u="1"/>
-        <n v="80976" u="1"/>
-        <n v="120584" u="1"/>
-        <n v="73656" u="1"/>
-        <n v="52916" u="1"/>
-        <n v="60516" u="1"/>
-        <n v="50480" u="1"/>
-        <n v="53196" u="1"/>
-        <n v="94568" u="1"/>
-        <n v="54012" u="1"/>
-        <n v="79928" u="1"/>
-        <n v="133364" u="1"/>
-        <n v="39232" u="1"/>
-        <n v="42216" u="1"/>
-        <n v="22100" u="1"/>
-        <n v="45748" u="1"/>
+        <n v="75860" u="1"/>
+        <n v="46436" u="1"/>
         <n v="66244" u="1"/>
-        <n v="82796" u="1"/>
-        <n v="24204" u="1"/>
-        <n v="58908" u="1"/>
-        <n v="204" u="1"/>
-        <n v="46436" u="1"/>
-        <n v="59188" u="1"/>
-        <n v="1540" u="1"/>
-        <n v="52544" u="1"/>
-        <n v="80792" u="1"/>
-        <n v="22992" u="1"/>
-        <n v="50516" u="1"/>
-        <n v="78088" u="1"/>
-        <n v="48080" u="1"/>
-        <n v="6888" u="1"/>
-        <n v="40760" u="1"/>
-        <n v="39408" u="1"/>
-        <n v="96972" u="1"/>
-        <n v="123828" u="1"/>
-        <n v="61520" u="1"/>
-        <n v="45516" u="1"/>
-        <n v="31956" u="1"/>
-        <n v="36028" u="1"/>
-        <n v="76784" u="1"/>
-        <n v="80584" u="1"/>
-        <n v="44444" u="1"/>
-        <n v="69744" u="1"/>
-        <n v="20708" u="1"/>
-        <n v="43512" u="1"/>
-        <n v="47720" u="1"/>
-        <n v="86740" u="1"/>
-        <n v="54912" u="1"/>
-        <n v="83896" u="1"/>
-        <n v="1932" u="1"/>
-        <n v="32516" u="1"/>
-        <n v="96112" u="1"/>
-        <n v="48408" u="1"/>
-        <n v="77532" u="1"/>
-        <n v="39864" u="1"/>
-        <n v="75364" u="1"/>
-        <n v="93268" u="1"/>
-        <n v="5692" u="1"/>
-        <n v="134028" u="1"/>
-        <n v="48420" u="1"/>
-        <n v="66576" u="1"/>
-        <n v="133516" u="1"/>
-        <n v="20184" u="1"/>
-        <n v="11232" u="1"/>
-        <n v="75272" u="1"/>
-        <n v="81520" u="1"/>
-        <n v="6288" u="1"/>
-        <n v="133844" u="1"/>
-        <n v="76648" u="1"/>
+        <n v="85840" u="1"/>
+        <n v="59520" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="THREADID" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="135232" maxValue="135232" count="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="135232" maxValue="139356" count="2">
         <n v="135232"/>
+        <n v="139356"/>
       </sharedItems>
     </cacheField>
     <cacheField name="EPOCH" numFmtId="0" sqlType="6">
@@ -4044,7 +4046,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="MSE_T" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.31871588528156E-2" maxValue="2.9612287878990201E-2"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="3.24953813105822E-3" maxValue="2.9612287878990201E-2"/>
     </cacheField>
     <cacheField name="MSE_V" numFmtId="0" sqlType="6">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="0" count="1">
@@ -4061,12 +4063,14 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="gcaglion" refreshedDate="43157.03268877315" createdVersion="6" refreshedVersion="5" minRefreshableVersion="3" recordCount="4320">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="gcaglion" refreshedDate="43157.040165740742" createdVersion="6" refreshedVersion="5" minRefreshableVersion="3" recordCount="485920">
   <cacheSource type="external" connectionId="3"/>
   <cacheFields count="15">
     <cacheField name="PROCESSID" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="204" maxValue="139476" count="179">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="204" maxValue="140228" count="181">
         <n v="43024"/>
+        <n v="140220"/>
+        <n v="140228"/>
         <n v="82796" u="1"/>
         <n v="57572" u="1"/>
         <n v="134852" u="1"/>
@@ -4248,8 +4252,10 @@
       </sharedItems>
     </cacheField>
     <cacheField name="THREADID" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="54988" maxValue="139660" count="5">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="54988" maxValue="139660" count="7">
         <n v="135232"/>
+        <n v="139356"/>
+        <n v="137012"/>
         <n v="54988" u="1"/>
         <n v="137352" u="1"/>
         <n v="139660" u="1"/>
@@ -4258,24 +4264,28 @@
     </cacheField>
     <cacheField name="SETID" numFmtId="0" sqlType="6">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="1" count="2">
+        <n v="1"/>
         <n v="0"/>
-        <n v="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="NETPROCESSID" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="43024" count="2">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="140228" count="4">
+        <n v="0"/>
         <n v="43024"/>
-        <n v="0"/>
+        <n v="140220"/>
+        <n v="140228"/>
       </sharedItems>
     </cacheField>
     <cacheField name="NETTHREADID" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="135232" count="2">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="139356" count="4">
+        <n v="0"/>
         <n v="135232"/>
-        <n v="0"/>
+        <n v="139356"/>
+        <n v="137012"/>
       </sharedItems>
     </cacheField>
     <cacheField name="POS" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="539"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="59799"/>
     </cacheField>
     <cacheField name="FEATUREID" numFmtId="0" sqlType="6">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="3" count="4">
@@ -4304,10 +4314,10 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-1.00000011920929" maxValue="1"/>
     </cacheField>
     <cacheField name="PREDICTEDTRS" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-0.84100401401519798" maxValue="0.81332200765609697"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-0.98163783550262496" maxValue="0.81332200765609697"/>
     </cacheField>
     <cacheField name="ERRORTRS" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="5.6892633438110399E-5" maxValue="1.3975193500518801"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2.2351741790771501E-8" maxValue="1.8223857879638701"/>
     </cacheField>
     <cacheField name="BARWIDTH" numFmtId="0" sqlType="6">
       <sharedItems containsString="0" containsBlank="1" count="1">
@@ -4329,195 +4339,197 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="53" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="60" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
   <location ref="A1:B52" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0">
-      <items count="179">
-        <item m="1" x="129"/>
-        <item m="1" x="86"/>
-        <item m="1" x="132"/>
-        <item m="1" x="158"/>
-        <item m="1" x="9"/>
-        <item m="1" x="5"/>
-        <item m="1" x="106"/>
-        <item m="1" x="99"/>
-        <item m="1" x="85"/>
-        <item m="1" x="166"/>
-        <item m="1" x="175"/>
-        <item m="1" x="15"/>
-        <item m="1" x="139"/>
-        <item m="1" x="104"/>
-        <item m="1" x="47"/>
-        <item m="1" x="172"/>
-        <item m="1" x="96"/>
-        <item m="1" x="73"/>
-        <item m="1" x="12"/>
-        <item m="1" x="60"/>
-        <item m="1" x="94"/>
-        <item m="1" x="44"/>
-        <item m="1" x="171"/>
-        <item m="1" x="152"/>
-        <item m="1" x="56"/>
-        <item m="1" x="70"/>
-        <item m="1" x="123"/>
-        <item m="1" x="64"/>
-        <item m="1" x="51"/>
-        <item m="1" x="135"/>
-        <item m="1" x="33"/>
-        <item m="1" x="20"/>
-        <item m="1" x="127"/>
-        <item m="1" x="68"/>
-        <item m="1" x="27"/>
-        <item m="1" x="11"/>
-        <item m="1" x="4"/>
-        <item m="1" x="36"/>
-        <item m="1" x="78"/>
-        <item m="1" x="13"/>
-        <item m="1" x="146"/>
-        <item m="1" x="159"/>
-        <item m="1" x="40"/>
-        <item m="1" x="109"/>
-        <item m="1" x="22"/>
-        <item m="1" x="58"/>
-        <item m="1" x="92"/>
-        <item m="1" x="42"/>
-        <item m="1" x="147"/>
-        <item m="1" x="2"/>
-        <item m="1" x="121"/>
-        <item m="1" x="141"/>
-        <item m="1" x="163"/>
-        <item m="1" x="140"/>
-        <item m="1" x="14"/>
-        <item m="1" x="17"/>
-        <item m="1" x="89"/>
-        <item m="1" x="122"/>
-        <item m="1" x="101"/>
-        <item x="0"/>
-        <item m="1" x="97"/>
-        <item m="1" x="69"/>
-        <item m="1" x="153"/>
-        <item m="1" x="57"/>
-        <item m="1" x="150"/>
-        <item m="1" x="45"/>
-        <item m="1" x="90"/>
-        <item m="1" x="145"/>
-        <item m="1" x="124"/>
-        <item m="1" x="130"/>
-        <item m="1" x="75"/>
-        <item m="1" x="72"/>
-        <item m="1" x="59"/>
-        <item m="1" x="71"/>
-        <item m="1" x="54"/>
-        <item m="1" x="154"/>
-        <item m="1" x="138"/>
-        <item m="1" x="30"/>
-        <item m="1" x="103"/>
-        <item m="1" x="18"/>
-        <item m="1" x="161"/>
-        <item m="1" x="168"/>
-        <item m="1" x="105"/>
-        <item m="1" x="55"/>
-        <item m="1" x="8"/>
-        <item m="1" x="115"/>
-        <item m="1" x="136"/>
-        <item m="1" x="133"/>
-        <item m="1" x="113"/>
-        <item m="1" x="116"/>
-        <item m="1" x="118"/>
-        <item m="1" x="156"/>
-        <item m="1" x="62"/>
-        <item m="1" x="21"/>
-        <item m="1" x="28"/>
-        <item m="1" x="128"/>
-        <item m="1" x="131"/>
-        <item m="1" x="82"/>
-        <item m="1" x="37"/>
-        <item m="1" x="100"/>
-        <item m="1" x="114"/>
-        <item m="1" x="144"/>
-        <item m="1" x="25"/>
-        <item m="1" x="102"/>
-        <item m="1" x="19"/>
-        <item m="1" x="125"/>
-        <item m="1" x="169"/>
-        <item m="1" x="66"/>
-        <item m="1" x="46"/>
-        <item m="1" x="10"/>
-        <item m="1" x="79"/>
-        <item m="1" x="151"/>
-        <item m="1" x="6"/>
-        <item m="1" x="24"/>
-        <item m="1" x="112"/>
-        <item m="1" x="173"/>
-        <item m="1" x="164"/>
-        <item m="1" x="32"/>
-        <item m="1" x="34"/>
-        <item m="1" x="49"/>
-        <item m="1" x="52"/>
-        <item m="1" x="177"/>
-        <item m="1" x="148"/>
-        <item m="1" x="91"/>
-        <item m="1" x="1"/>
-        <item m="1" x="162"/>
-        <item m="1" x="63"/>
-        <item m="1" x="61"/>
-        <item m="1" x="31"/>
-        <item m="1" x="137"/>
-        <item m="1" x="81"/>
-        <item m="1" x="3"/>
-        <item m="1" x="26"/>
-        <item m="1" x="29"/>
-        <item m="1" x="87"/>
-        <item m="1" x="119"/>
-        <item m="1" x="149"/>
-        <item m="1" x="39"/>
-        <item m="1" x="43"/>
-        <item m="1" x="134"/>
-        <item m="1" x="110"/>
-        <item m="1" x="53"/>
-        <item m="1" x="174"/>
-        <item m="1" x="7"/>
-        <item m="1" x="126"/>
-        <item m="1" x="108"/>
-        <item m="1" x="157"/>
-        <item m="1" x="95"/>
-        <item m="1" x="107"/>
-        <item m="1" x="16"/>
-        <item m="1" x="48"/>
-        <item m="1" x="155"/>
-        <item m="1" x="83"/>
-        <item m="1" x="98"/>
-        <item m="1" x="50"/>
-        <item m="1" x="76"/>
-        <item m="1" x="38"/>
-        <item m="1" x="67"/>
-        <item m="1" x="41"/>
-        <item m="1" x="165"/>
-        <item m="1" x="117"/>
-        <item m="1" x="160"/>
-        <item m="1" x="93"/>
-        <item m="1" x="142"/>
-        <item m="1" x="84"/>
-        <item m="1" x="77"/>
-        <item m="1" x="23"/>
-        <item m="1" x="74"/>
-        <item m="1" x="111"/>
-        <item m="1" x="88"/>
-        <item m="1" x="143"/>
-        <item m="1" x="65"/>
-        <item m="1" x="35"/>
-        <item m="1" x="120"/>
-        <item m="1" x="170"/>
-        <item m="1" x="176"/>
-        <item m="1" x="80"/>
-        <item m="1" x="167"/>
+      <items count="180">
+        <item h="1" m="1" x="42"/>
+        <item h="1" m="1" x="64"/>
+        <item h="1" m="1" x="61"/>
+        <item h="1" m="1" x="5"/>
+        <item h="1" m="1" x="78"/>
+        <item h="1" m="1" x="167"/>
+        <item h="1" m="1" x="39"/>
+        <item h="1" m="1" x="161"/>
+        <item h="1" m="1" x="79"/>
+        <item h="1" m="1" x="50"/>
+        <item h="1" m="1" x="44"/>
+        <item h="1" m="1" x="49"/>
+        <item h="1" m="1" x="116"/>
+        <item h="1" m="1" x="142"/>
+        <item h="1" m="1" x="6"/>
+        <item h="1" m="1" x="171"/>
+        <item h="1" m="1" x="102"/>
+        <item h="1" m="1" x="37"/>
+        <item h="1" m="1" x="22"/>
+        <item h="1" m="1" x="21"/>
+        <item h="1" m="1" x="65"/>
+        <item h="1" m="1" x="23"/>
+        <item h="1" m="1" x="67"/>
+        <item h="1" m="1" x="125"/>
+        <item h="1" m="1" x="40"/>
+        <item h="1" m="1" x="143"/>
+        <item h="1" m="1" x="92"/>
+        <item h="1" m="1" x="158"/>
+        <item h="1" m="1" x="80"/>
+        <item h="1" m="1" x="103"/>
+        <item h="1" m="1" x="85"/>
+        <item h="1" m="1" x="168"/>
+        <item h="1" m="1" x="13"/>
+        <item h="1" m="1" x="152"/>
+        <item h="1" m="1" x="53"/>
+        <item h="1" m="1" x="45"/>
+        <item h="1" m="1" x="68"/>
+        <item h="1" m="1" x="114"/>
+        <item h="1" m="1" x="14"/>
+        <item h="1" m="1" x="169"/>
+        <item h="1" m="1" x="133"/>
+        <item h="1" m="1" x="107"/>
+        <item h="1" m="1" x="31"/>
+        <item h="1" m="1" x="83"/>
+        <item h="1" m="1" x="54"/>
+        <item h="1" m="1" x="172"/>
+        <item h="1" m="1" x="104"/>
+        <item h="1" m="1" x="32"/>
+        <item h="1" m="1" x="7"/>
+        <item h="1" m="1" x="86"/>
+        <item h="1" m="1" x="17"/>
+        <item h="1" m="1" x="69"/>
+        <item h="1" m="1" x="170"/>
+        <item h="1" m="1" x="129"/>
+        <item h="1" m="1" x="97"/>
+        <item h="1" m="1" x="70"/>
+        <item h="1" m="1" x="173"/>
+        <item h="1" m="1" x="2"/>
+        <item h="1" m="1" x="73"/>
+        <item h="1" x="0"/>
+        <item h="1" m="1" x="43"/>
+        <item h="1" m="1" x="153"/>
+        <item h="1" m="1" x="18"/>
+        <item h="1" m="1" x="24"/>
+        <item h="1" m="1" x="28"/>
+        <item h="1" m="1" x="15"/>
+        <item h="1" m="1" x="144"/>
+        <item h="1" m="1" x="55"/>
+        <item h="1" m="1" x="154"/>
+        <item h="1" m="1" x="175"/>
+        <item h="1" m="1" x="33"/>
+        <item h="1" m="1" x="126"/>
+        <item h="1" m="1" x="41"/>
+        <item h="1" m="1" x="98"/>
+        <item h="1" m="1" x="109"/>
+        <item h="1" m="1" x="118"/>
+        <item h="1" m="1" x="165"/>
+        <item h="1" m="1" x="99"/>
+        <item h="1" m="1" x="105"/>
+        <item h="1" m="1" x="19"/>
+        <item h="1" m="1" x="127"/>
+        <item h="1" m="1" x="29"/>
+        <item h="1" m="1" x="57"/>
+        <item h="1" m="1" x="11"/>
+        <item h="1" m="1" x="145"/>
+        <item h="1" m="1" x="112"/>
+        <item h="1" m="1" x="138"/>
+        <item h="1" m="1" x="149"/>
+        <item h="1" m="1" x="95"/>
+        <item h="1" m="1" x="122"/>
+        <item h="1" m="1" x="89"/>
+        <item h="1" m="1" x="25"/>
+        <item h="1" m="1" x="162"/>
+        <item h="1" m="1" x="4"/>
+        <item h="1" m="1" x="87"/>
+        <item h="1" m="1" x="27"/>
+        <item h="1" m="1" x="58"/>
+        <item h="1" m="1" x="34"/>
+        <item h="1" m="1" x="178"/>
+        <item h="1" m="1" x="16"/>
+        <item h="1" m="1" x="155"/>
+        <item h="1" m="1" x="62"/>
+        <item h="1" m="1" x="150"/>
+        <item h="1" m="1" x="51"/>
+        <item h="1" m="1" x="139"/>
+        <item h="1" m="1" x="176"/>
+        <item h="1" m="1" x="130"/>
+        <item h="1" m="1" x="74"/>
+        <item h="1" m="1" x="90"/>
+        <item h="1" m="1" x="134"/>
+        <item h="1" m="1" x="159"/>
+        <item h="1" m="1" x="120"/>
+        <item h="1" m="1" x="136"/>
+        <item h="1" m="1" x="81"/>
+        <item h="1" m="1" x="47"/>
+        <item h="1" m="1" x="75"/>
+        <item h="1" m="1" x="35"/>
+        <item h="1" m="1" x="174"/>
+        <item h="1" m="1" x="91"/>
+        <item h="1" m="1" x="137"/>
+        <item h="1" m="1" x="166"/>
+        <item h="1" m="1" x="96"/>
+        <item h="1" m="1" x="36"/>
+        <item h="1" m="1" x="140"/>
+        <item h="1" m="1" x="71"/>
+        <item h="1" m="1" x="124"/>
+        <item h="1" m="1" x="123"/>
+        <item h="1" m="1" x="151"/>
+        <item h="1" m="1" x="93"/>
+        <item h="1" m="1" x="8"/>
+        <item h="1" m="1" x="82"/>
+        <item h="1" m="1" x="52"/>
+        <item h="1" m="1" x="160"/>
+        <item h="1" m="1" x="100"/>
+        <item h="1" m="1" x="128"/>
+        <item h="1" m="1" x="119"/>
+        <item h="1" m="1" x="94"/>
+        <item h="1" m="1" x="26"/>
+        <item h="1" m="1" x="101"/>
+        <item h="1" m="1" x="63"/>
+        <item h="1" m="1" x="146"/>
+        <item h="1" m="1" x="110"/>
+        <item h="1" m="1" x="76"/>
+        <item h="1" m="1" x="66"/>
+        <item h="1" m="1" x="3"/>
+        <item h="1" m="1" x="20"/>
+        <item h="1" m="1" x="156"/>
+        <item h="1" m="1" x="9"/>
+        <item h="1" m="1" x="77"/>
+        <item h="1" m="1" x="106"/>
+        <item h="1" m="1" x="177"/>
+        <item h="1" m="1" x="131"/>
+        <item h="1" m="1" x="163"/>
+        <item h="1" m="1" x="60"/>
+        <item h="1" m="1" x="147"/>
+        <item h="1" m="1" x="38"/>
+        <item h="1" m="1" x="113"/>
+        <item h="1" m="1" x="121"/>
+        <item h="1" m="1" x="10"/>
+        <item h="1" m="1" x="157"/>
+        <item h="1" m="1" x="141"/>
+        <item h="1" m="1" x="132"/>
+        <item h="1" m="1" x="115"/>
+        <item h="1" m="1" x="108"/>
+        <item h="1" m="1" x="88"/>
+        <item h="1" m="1" x="56"/>
+        <item h="1" m="1" x="148"/>
+        <item h="1" m="1" x="46"/>
+        <item h="1" m="1" x="111"/>
+        <item h="1" m="1" x="12"/>
+        <item h="1" m="1" x="117"/>
+        <item h="1" m="1" x="135"/>
+        <item h="1" m="1" x="48"/>
+        <item h="1" m="1" x="59"/>
+        <item h="1" m="1" x="84"/>
+        <item h="1" m="1" x="72"/>
+        <item h="1" m="1" x="164"/>
+        <item h="1" m="1" x="30"/>
+        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0">
-      <items count="2">
+      <items count="3">
         <item x="0"/>
+        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -5311,206 +5323,210 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="57" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="64" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" fieldListSortAscending="1">
   <location ref="A3:C10" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField axis="axisCol" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
-      <items count="179">
-        <item m="1" x="4"/>
-        <item m="1" x="82"/>
-        <item m="1" x="168"/>
-        <item m="1" x="49"/>
-        <item m="1" x="120"/>
-        <item m="1" x="148"/>
-        <item m="1" x="70"/>
-        <item m="1" x="130"/>
-        <item m="1" x="94"/>
-        <item m="1" x="160"/>
-        <item m="1" x="83"/>
-        <item m="1" x="86"/>
-        <item m="1" x="169"/>
-        <item m="1" x="60"/>
-        <item m="1" x="146"/>
-        <item m="1" x="128"/>
-        <item m="1" x="84"/>
-        <item m="1" x="44"/>
-        <item m="1" x="69"/>
-        <item m="1" x="64"/>
-        <item m="1" x="40"/>
-        <item m="1" x="164"/>
-        <item m="1" x="54"/>
-        <item m="1" x="53"/>
-        <item m="1" x="6"/>
-        <item m="1" x="172"/>
-        <item m="1" x="107"/>
-        <item m="1" x="39"/>
-        <item m="1" x="22"/>
-        <item m="1" x="23"/>
-        <item m="1" x="73"/>
-        <item m="1" x="41"/>
-        <item m="1" x="108"/>
-        <item m="1" x="12"/>
-        <item m="1" x="154"/>
-        <item m="1" x="57"/>
-        <item m="1" x="50"/>
-        <item m="1" x="74"/>
-        <item m="1" x="119"/>
-        <item m="1" x="170"/>
-        <item m="1" x="137"/>
-        <item m="1" x="112"/>
-        <item m="1" x="33"/>
-        <item m="1" x="58"/>
-        <item m="1" x="109"/>
-        <item m="1" x="34"/>
-        <item m="1" x="7"/>
-        <item m="1" x="87"/>
-        <item m="1" x="15"/>
-        <item m="1" x="75"/>
-        <item m="1" x="171"/>
-        <item m="1" x="134"/>
-        <item m="1" x="76"/>
-        <item m="1" x="173"/>
-        <item m="1" x="77"/>
-        <item m="1" x="45"/>
-        <item m="1" x="155"/>
-        <item m="1" x="17"/>
-        <item m="1" x="24"/>
-        <item m="1" x="29"/>
-        <item m="1" x="13"/>
-        <item m="1" x="149"/>
-        <item m="1" x="59"/>
-        <item m="1" x="176"/>
-        <item m="1" x="35"/>
-        <item m="1" x="131"/>
-        <item m="1" x="42"/>
-        <item m="1" x="101"/>
-        <item m="1" x="114"/>
-        <item m="1" x="123"/>
-        <item m="1" x="166"/>
-        <item m="1" x="102"/>
-        <item m="1" x="110"/>
-        <item m="1" x="18"/>
-        <item m="1" x="132"/>
-        <item m="1" x="30"/>
-        <item m="1" x="150"/>
-        <item m="1" x="118"/>
-        <item m="1" x="144"/>
-        <item m="1" x="99"/>
-        <item m="1" x="127"/>
-        <item m="1" x="92"/>
-        <item m="1" x="25"/>
-        <item m="1" x="165"/>
-        <item m="1" x="2"/>
-        <item m="1" x="88"/>
-        <item m="1" x="27"/>
-        <item m="1" x="36"/>
-        <item m="1" x="177"/>
-        <item m="1" x="156"/>
-        <item m="1" x="65"/>
-        <item m="1" x="152"/>
-        <item m="1" x="55"/>
-        <item m="1" x="145"/>
-        <item m="1" x="135"/>
-        <item m="1" x="78"/>
-        <item m="1" x="93"/>
-        <item m="1" x="138"/>
-        <item m="1" x="161"/>
-        <item m="1" x="125"/>
-        <item m="1" x="139"/>
-        <item m="1" x="51"/>
-        <item m="1" x="79"/>
-        <item m="1" x="174"/>
-        <item m="1" x="140"/>
-        <item m="1" x="37"/>
-        <item m="1" x="153"/>
-        <item m="1" x="56"/>
-        <item m="1" x="162"/>
-        <item m="1" x="124"/>
-        <item m="1" x="97"/>
-        <item m="1" x="26"/>
-        <item m="1" x="104"/>
-        <item m="1" x="80"/>
-        <item m="1" x="71"/>
-        <item m="1" x="1"/>
-        <item m="1" x="19"/>
-        <item m="1" x="8"/>
-        <item m="1" x="81"/>
-        <item m="1" x="111"/>
-        <item m="1" x="63"/>
-        <item m="1" x="151"/>
-        <item m="1" x="9"/>
-        <item m="1" x="157"/>
-        <item m="1" x="147"/>
-        <item m="1" x="113"/>
-        <item m="1" x="89"/>
-        <item m="1" x="175"/>
-        <item m="1" x="136"/>
-        <item m="1" x="129"/>
-        <item m="1" x="32"/>
-        <item m="1" x="142"/>
-        <item m="1" x="72"/>
-        <item m="1" x="121"/>
-        <item m="1" x="116"/>
-        <item m="1" x="95"/>
-        <item m="1" x="90"/>
-        <item m="1" x="158"/>
-        <item m="1" x="62"/>
-        <item m="1" x="122"/>
-        <item m="1" x="143"/>
-        <item m="1" x="117"/>
-        <item m="1" x="61"/>
-        <item m="1" x="163"/>
-        <item m="1" x="16"/>
-        <item m="1" x="66"/>
-        <item m="1" x="67"/>
-        <item m="1" x="85"/>
-        <item m="1" x="31"/>
-        <item m="1" x="167"/>
-        <item m="1" x="178"/>
-        <item m="1" x="11"/>
-        <item m="1" x="100"/>
-        <item m="1" x="21"/>
-        <item m="1" x="91"/>
-        <item m="1" x="105"/>
-        <item m="1" x="10"/>
-        <item m="1" x="159"/>
-        <item m="1" x="48"/>
-        <item m="1" x="68"/>
-        <item m="1" x="20"/>
-        <item m="1" x="141"/>
-        <item m="1" x="3"/>
-        <item m="1" x="133"/>
-        <item m="1" x="43"/>
-        <item m="1" x="28"/>
-        <item m="1" x="14"/>
-        <item m="1" x="46"/>
-        <item m="1" x="103"/>
-        <item m="1" x="96"/>
-        <item m="1" x="47"/>
-        <item m="1" x="106"/>
-        <item m="1" x="52"/>
-        <item m="1" x="126"/>
-        <item m="1" x="98"/>
-        <item m="1" x="115"/>
-        <item m="1" x="5"/>
-        <item m="1" x="38"/>
+      <items count="181">
+        <item h="1" m="1" x="6"/>
+        <item h="1" m="1" x="84"/>
+        <item h="1" m="1" x="170"/>
+        <item h="1" m="1" x="51"/>
+        <item h="1" m="1" x="122"/>
+        <item h="1" m="1" x="150"/>
+        <item h="1" m="1" x="72"/>
+        <item h="1" m="1" x="132"/>
+        <item h="1" m="1" x="96"/>
+        <item h="1" m="1" x="162"/>
+        <item h="1" m="1" x="85"/>
+        <item h="1" m="1" x="88"/>
+        <item h="1" m="1" x="171"/>
+        <item h="1" m="1" x="62"/>
+        <item h="1" m="1" x="148"/>
+        <item h="1" m="1" x="130"/>
+        <item h="1" m="1" x="86"/>
+        <item h="1" m="1" x="46"/>
+        <item h="1" m="1" x="71"/>
+        <item h="1" m="1" x="66"/>
+        <item h="1" m="1" x="42"/>
+        <item h="1" m="1" x="166"/>
+        <item h="1" m="1" x="56"/>
+        <item h="1" m="1" x="55"/>
+        <item h="1" m="1" x="8"/>
+        <item h="1" m="1" x="174"/>
+        <item h="1" m="1" x="109"/>
+        <item h="1" m="1" x="41"/>
+        <item h="1" m="1" x="24"/>
+        <item h="1" m="1" x="25"/>
+        <item h="1" m="1" x="75"/>
+        <item h="1" m="1" x="43"/>
+        <item h="1" m="1" x="110"/>
+        <item h="1" m="1" x="14"/>
+        <item h="1" m="1" x="156"/>
+        <item h="1" m="1" x="59"/>
+        <item h="1" m="1" x="52"/>
+        <item h="1" m="1" x="76"/>
+        <item h="1" m="1" x="121"/>
+        <item h="1" m="1" x="172"/>
+        <item h="1" m="1" x="139"/>
+        <item h="1" m="1" x="114"/>
+        <item h="1" m="1" x="35"/>
+        <item h="1" m="1" x="60"/>
+        <item h="1" m="1" x="111"/>
+        <item h="1" m="1" x="36"/>
+        <item h="1" m="1" x="9"/>
+        <item h="1" m="1" x="89"/>
+        <item h="1" m="1" x="17"/>
+        <item h="1" m="1" x="77"/>
+        <item h="1" m="1" x="173"/>
+        <item h="1" m="1" x="136"/>
+        <item h="1" m="1" x="78"/>
+        <item h="1" m="1" x="175"/>
+        <item h="1" m="1" x="79"/>
+        <item h="1" m="1" x="47"/>
+        <item h="1" m="1" x="157"/>
+        <item h="1" m="1" x="19"/>
+        <item h="1" m="1" x="26"/>
+        <item h="1" m="1" x="31"/>
+        <item h="1" m="1" x="15"/>
+        <item h="1" m="1" x="151"/>
+        <item h="1" m="1" x="61"/>
+        <item h="1" m="1" x="178"/>
+        <item h="1" m="1" x="37"/>
+        <item h="1" m="1" x="133"/>
+        <item h="1" m="1" x="44"/>
+        <item h="1" m="1" x="103"/>
+        <item h="1" m="1" x="116"/>
+        <item h="1" m="1" x="125"/>
+        <item h="1" m="1" x="168"/>
+        <item h="1" m="1" x="104"/>
+        <item h="1" m="1" x="112"/>
+        <item h="1" m="1" x="20"/>
+        <item h="1" m="1" x="134"/>
+        <item h="1" m="1" x="32"/>
+        <item h="1" m="1" x="152"/>
+        <item h="1" m="1" x="120"/>
+        <item h="1" m="1" x="146"/>
+        <item h="1" m="1" x="101"/>
+        <item h="1" m="1" x="129"/>
+        <item h="1" m="1" x="94"/>
+        <item h="1" m="1" x="27"/>
+        <item h="1" m="1" x="167"/>
+        <item h="1" m="1" x="4"/>
+        <item h="1" m="1" x="90"/>
+        <item h="1" m="1" x="29"/>
+        <item h="1" m="1" x="38"/>
+        <item h="1" m="1" x="179"/>
+        <item h="1" m="1" x="158"/>
+        <item h="1" m="1" x="67"/>
+        <item h="1" m="1" x="154"/>
+        <item h="1" m="1" x="57"/>
+        <item h="1" m="1" x="147"/>
+        <item h="1" m="1" x="137"/>
+        <item h="1" m="1" x="80"/>
+        <item h="1" m="1" x="95"/>
+        <item h="1" m="1" x="140"/>
+        <item h="1" m="1" x="163"/>
+        <item h="1" m="1" x="127"/>
+        <item h="1" m="1" x="141"/>
+        <item h="1" m="1" x="53"/>
+        <item h="1" m="1" x="81"/>
+        <item h="1" m="1" x="176"/>
+        <item h="1" m="1" x="142"/>
+        <item h="1" m="1" x="39"/>
+        <item h="1" m="1" x="155"/>
+        <item h="1" m="1" x="58"/>
+        <item h="1" m="1" x="164"/>
+        <item h="1" m="1" x="126"/>
+        <item h="1" m="1" x="99"/>
+        <item h="1" m="1" x="28"/>
+        <item h="1" m="1" x="106"/>
+        <item h="1" m="1" x="82"/>
+        <item h="1" m="1" x="73"/>
+        <item h="1" m="1" x="3"/>
+        <item h="1" m="1" x="21"/>
+        <item h="1" m="1" x="10"/>
+        <item h="1" m="1" x="83"/>
+        <item h="1" m="1" x="113"/>
+        <item h="1" m="1" x="65"/>
+        <item h="1" m="1" x="153"/>
+        <item h="1" m="1" x="11"/>
+        <item h="1" m="1" x="159"/>
+        <item h="1" m="1" x="149"/>
+        <item h="1" m="1" x="115"/>
+        <item h="1" m="1" x="91"/>
+        <item h="1" m="1" x="177"/>
+        <item h="1" m="1" x="138"/>
+        <item h="1" m="1" x="131"/>
+        <item h="1" m="1" x="34"/>
+        <item h="1" m="1" x="144"/>
+        <item h="1" m="1" x="74"/>
+        <item h="1" m="1" x="123"/>
+        <item h="1" m="1" x="118"/>
+        <item h="1" m="1" x="97"/>
+        <item h="1" m="1" x="92"/>
+        <item h="1" m="1" x="160"/>
+        <item h="1" m="1" x="64"/>
+        <item h="1" m="1" x="124"/>
+        <item h="1" m="1" x="145"/>
+        <item h="1" m="1" x="119"/>
+        <item h="1" m="1" x="63"/>
+        <item h="1" m="1" x="165"/>
+        <item h="1" m="1" x="18"/>
+        <item h="1" m="1" x="68"/>
+        <item h="1" m="1" x="69"/>
+        <item h="1" m="1" x="87"/>
+        <item h="1" m="1" x="33"/>
+        <item h="1" m="1" x="169"/>
+        <item h="1" m="1" x="180"/>
+        <item h="1" m="1" x="13"/>
+        <item h="1" m="1" x="102"/>
+        <item h="1" m="1" x="23"/>
+        <item h="1" m="1" x="93"/>
+        <item h="1" m="1" x="107"/>
+        <item h="1" m="1" x="12"/>
+        <item h="1" m="1" x="161"/>
+        <item h="1" m="1" x="50"/>
+        <item h="1" m="1" x="70"/>
+        <item h="1" m="1" x="22"/>
+        <item h="1" m="1" x="143"/>
+        <item h="1" m="1" x="5"/>
+        <item h="1" m="1" x="135"/>
+        <item h="1" m="1" x="45"/>
+        <item h="1" m="1" x="30"/>
+        <item h="1" m="1" x="16"/>
+        <item h="1" m="1" x="48"/>
+        <item h="1" m="1" x="105"/>
+        <item h="1" m="1" x="98"/>
+        <item h="1" m="1" x="49"/>
+        <item h="1" m="1" x="108"/>
+        <item h="1" m="1" x="54"/>
+        <item h="1" m="1" x="128"/>
+        <item h="1" m="1" x="100"/>
+        <item h="1" m="1" x="117"/>
+        <item h="1" m="1" x="7"/>
+        <item h="1" m="1" x="40"/>
         <item x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
       </items>
     </pivotField>
     <pivotField axis="axisCol" showAll="0">
-      <items count="6">
-        <item m="1" x="2"/>
-        <item m="1" x="1"/>
+      <items count="8">
         <item m="1" x="4"/>
         <item m="1" x="3"/>
+        <item m="1" x="6"/>
+        <item m="1" x="5"/>
         <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0" defaultSubtotal="0">
       <items count="2">
+        <item h="1" x="1"/>
         <item x="0"/>
-        <item h="1" x="1"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
@@ -6092,185 +6108,186 @@
   </pivotTables>
   <data>
     <tabular pivotCacheId="1">
-      <items count="178">
-        <i x="0" s="1"/>
-        <i x="129" s="1" nd="1"/>
-        <i x="86" s="1" nd="1"/>
-        <i x="132" s="1" nd="1"/>
-        <i x="158" s="1" nd="1"/>
-        <i x="9" s="1" nd="1"/>
-        <i x="5" s="1" nd="1"/>
-        <i x="106" s="1" nd="1"/>
-        <i x="99" s="1" nd="1"/>
-        <i x="85" s="1" nd="1"/>
-        <i x="166" s="1" nd="1"/>
-        <i x="175" s="1" nd="1"/>
-        <i x="15" s="1" nd="1"/>
-        <i x="139" s="1" nd="1"/>
-        <i x="104" s="1" nd="1"/>
-        <i x="47" s="1" nd="1"/>
-        <i x="172" s="1" nd="1"/>
-        <i x="96" s="1" nd="1"/>
-        <i x="73" s="1" nd="1"/>
-        <i x="12" s="1" nd="1"/>
-        <i x="60" s="1" nd="1"/>
-        <i x="94" s="1" nd="1"/>
-        <i x="44" s="1" nd="1"/>
-        <i x="171" s="1" nd="1"/>
-        <i x="152" s="1" nd="1"/>
-        <i x="56" s="1" nd="1"/>
-        <i x="70" s="1" nd="1"/>
-        <i x="123" s="1" nd="1"/>
-        <i x="64" s="1" nd="1"/>
-        <i x="51" s="1" nd="1"/>
-        <i x="135" s="1" nd="1"/>
-        <i x="33" s="1" nd="1"/>
-        <i x="20" s="1" nd="1"/>
-        <i x="127" s="1" nd="1"/>
-        <i x="68" s="1" nd="1"/>
-        <i x="27" s="1" nd="1"/>
-        <i x="11" s="1" nd="1"/>
-        <i x="4" s="1" nd="1"/>
-        <i x="36" s="1" nd="1"/>
-        <i x="78" s="1" nd="1"/>
-        <i x="13" s="1" nd="1"/>
-        <i x="146" s="1" nd="1"/>
-        <i x="159" s="1" nd="1"/>
-        <i x="40" s="1" nd="1"/>
-        <i x="109" s="1" nd="1"/>
-        <i x="22" s="1" nd="1"/>
-        <i x="58" s="1" nd="1"/>
-        <i x="92" s="1" nd="1"/>
-        <i x="42" s="1" nd="1"/>
-        <i x="147" s="1" nd="1"/>
-        <i x="2" s="1" nd="1"/>
-        <i x="121" s="1" nd="1"/>
-        <i x="141" s="1" nd="1"/>
-        <i x="163" s="1" nd="1"/>
-        <i x="140" s="1" nd="1"/>
-        <i x="14" s="1" nd="1"/>
-        <i x="17" s="1" nd="1"/>
-        <i x="89" s="1" nd="1"/>
-        <i x="122" s="1" nd="1"/>
-        <i x="101" s="1" nd="1"/>
-        <i x="97" s="1" nd="1"/>
-        <i x="69" s="1" nd="1"/>
-        <i x="153" s="1" nd="1"/>
-        <i x="57" s="1" nd="1"/>
-        <i x="150" s="1" nd="1"/>
-        <i x="45" s="1" nd="1"/>
-        <i x="90" s="1" nd="1"/>
-        <i x="145" s="1" nd="1"/>
-        <i x="124" s="1" nd="1"/>
-        <i x="130" s="1" nd="1"/>
-        <i x="75" s="1" nd="1"/>
-        <i x="72" s="1" nd="1"/>
-        <i x="59" s="1" nd="1"/>
-        <i x="71" s="1" nd="1"/>
-        <i x="54" s="1" nd="1"/>
-        <i x="154" s="1" nd="1"/>
-        <i x="138" s="1" nd="1"/>
-        <i x="30" s="1" nd="1"/>
-        <i x="103" s="1" nd="1"/>
-        <i x="18" s="1" nd="1"/>
-        <i x="161" s="1" nd="1"/>
-        <i x="168" s="1" nd="1"/>
-        <i x="105" s="1" nd="1"/>
-        <i x="55" s="1" nd="1"/>
-        <i x="8" s="1" nd="1"/>
-        <i x="115" s="1" nd="1"/>
-        <i x="136" s="1" nd="1"/>
-        <i x="133" s="1" nd="1"/>
-        <i x="113" s="1" nd="1"/>
-        <i x="116" s="1" nd="1"/>
-        <i x="118" s="1" nd="1"/>
-        <i x="156" s="1" nd="1"/>
-        <i x="62" s="1" nd="1"/>
-        <i x="21" s="1" nd="1"/>
-        <i x="28" s="1" nd="1"/>
-        <i x="128" s="1" nd="1"/>
-        <i x="131" s="1" nd="1"/>
-        <i x="82" s="1" nd="1"/>
-        <i x="37" s="1" nd="1"/>
-        <i x="100" s="1" nd="1"/>
-        <i x="114" s="1" nd="1"/>
-        <i x="144" s="1" nd="1"/>
-        <i x="25" s="1" nd="1"/>
-        <i x="102" s="1" nd="1"/>
-        <i x="19" s="1" nd="1"/>
-        <i x="125" s="1" nd="1"/>
-        <i x="169" s="1" nd="1"/>
-        <i x="66" s="1" nd="1"/>
-        <i x="46" s="1" nd="1"/>
-        <i x="10" s="1" nd="1"/>
-        <i x="79" s="1" nd="1"/>
-        <i x="151" s="1" nd="1"/>
-        <i x="6" s="1" nd="1"/>
-        <i x="24" s="1" nd="1"/>
-        <i x="112" s="1" nd="1"/>
-        <i x="173" s="1" nd="1"/>
-        <i x="164" s="1" nd="1"/>
-        <i x="32" s="1" nd="1"/>
-        <i x="34" s="1" nd="1"/>
-        <i x="49" s="1" nd="1"/>
-        <i x="52" s="1" nd="1"/>
-        <i x="177" s="1" nd="1"/>
-        <i x="148" s="1" nd="1"/>
-        <i x="91" s="1" nd="1"/>
-        <i x="1" s="1" nd="1"/>
-        <i x="162" s="1" nd="1"/>
-        <i x="63" s="1" nd="1"/>
-        <i x="61" s="1" nd="1"/>
-        <i x="31" s="1" nd="1"/>
-        <i x="137" s="1" nd="1"/>
-        <i x="81" s="1" nd="1"/>
-        <i x="3" s="1" nd="1"/>
-        <i x="26" s="1" nd="1"/>
-        <i x="29" s="1" nd="1"/>
-        <i x="87" s="1" nd="1"/>
-        <i x="119" s="1" nd="1"/>
-        <i x="149" s="1" nd="1"/>
-        <i x="39" s="1" nd="1"/>
-        <i x="43" s="1" nd="1"/>
-        <i x="134" s="1" nd="1"/>
-        <i x="110" s="1" nd="1"/>
-        <i x="53" s="1" nd="1"/>
-        <i x="174" s="1" nd="1"/>
-        <i x="7" s="1" nd="1"/>
-        <i x="126" s="1" nd="1"/>
-        <i x="108" s="1" nd="1"/>
-        <i x="157" s="1" nd="1"/>
-        <i x="95" s="1" nd="1"/>
-        <i x="107" s="1" nd="1"/>
-        <i x="16" s="1" nd="1"/>
-        <i x="48" s="1" nd="1"/>
-        <i x="155" s="1" nd="1"/>
-        <i x="83" s="1" nd="1"/>
-        <i x="98" s="1" nd="1"/>
-        <i x="50" s="1" nd="1"/>
-        <i x="76" s="1" nd="1"/>
-        <i x="38" s="1" nd="1"/>
-        <i x="67" s="1" nd="1"/>
-        <i x="41" s="1" nd="1"/>
-        <i x="165" s="1" nd="1"/>
-        <i x="117" s="1" nd="1"/>
-        <i x="160" s="1" nd="1"/>
-        <i x="93" s="1" nd="1"/>
-        <i x="142" s="1" nd="1"/>
-        <i x="84" s="1" nd="1"/>
-        <i x="77" s="1" nd="1"/>
-        <i x="23" s="1" nd="1"/>
-        <i x="74" s="1" nd="1"/>
-        <i x="111" s="1" nd="1"/>
-        <i x="88" s="1" nd="1"/>
-        <i x="143" s="1" nd="1"/>
-        <i x="65" s="1" nd="1"/>
-        <i x="35" s="1" nd="1"/>
-        <i x="120" s="1" nd="1"/>
-        <i x="170" s="1" nd="1"/>
-        <i x="176" s="1" nd="1"/>
-        <i x="80" s="1" nd="1"/>
-        <i x="167" s="1" nd="1"/>
+      <items count="179">
+        <i x="0"/>
+        <i x="1" s="1"/>
+        <i x="42" nd="1"/>
+        <i x="64" nd="1"/>
+        <i x="61" nd="1"/>
+        <i x="5" nd="1"/>
+        <i x="78" nd="1"/>
+        <i x="167" nd="1"/>
+        <i x="39" nd="1"/>
+        <i x="161" nd="1"/>
+        <i x="79" nd="1"/>
+        <i x="50" nd="1"/>
+        <i x="44" nd="1"/>
+        <i x="49" nd="1"/>
+        <i x="116" nd="1"/>
+        <i x="142" nd="1"/>
+        <i x="6" nd="1"/>
+        <i x="171" nd="1"/>
+        <i x="102" nd="1"/>
+        <i x="37" nd="1"/>
+        <i x="22" nd="1"/>
+        <i x="21" nd="1"/>
+        <i x="65" nd="1"/>
+        <i x="23" nd="1"/>
+        <i x="67" nd="1"/>
+        <i x="125" nd="1"/>
+        <i x="40" nd="1"/>
+        <i x="143" nd="1"/>
+        <i x="92" nd="1"/>
+        <i x="158" nd="1"/>
+        <i x="80" nd="1"/>
+        <i x="103" nd="1"/>
+        <i x="85" nd="1"/>
+        <i x="168" nd="1"/>
+        <i x="13" nd="1"/>
+        <i x="152" nd="1"/>
+        <i x="53" nd="1"/>
+        <i x="45" nd="1"/>
+        <i x="68" nd="1"/>
+        <i x="114" nd="1"/>
+        <i x="14" nd="1"/>
+        <i x="169" nd="1"/>
+        <i x="133" nd="1"/>
+        <i x="107" nd="1"/>
+        <i x="31" nd="1"/>
+        <i x="83" nd="1"/>
+        <i x="54" nd="1"/>
+        <i x="172" nd="1"/>
+        <i x="104" nd="1"/>
+        <i x="32" nd="1"/>
+        <i x="7" nd="1"/>
+        <i x="86" nd="1"/>
+        <i x="17" nd="1"/>
+        <i x="69" nd="1"/>
+        <i x="170" nd="1"/>
+        <i x="129" nd="1"/>
+        <i x="97" nd="1"/>
+        <i x="70" nd="1"/>
+        <i x="173" nd="1"/>
+        <i x="2" nd="1"/>
+        <i x="73" nd="1"/>
+        <i x="43" nd="1"/>
+        <i x="153" nd="1"/>
+        <i x="18" nd="1"/>
+        <i x="24" nd="1"/>
+        <i x="28" nd="1"/>
+        <i x="15" nd="1"/>
+        <i x="144" nd="1"/>
+        <i x="55" nd="1"/>
+        <i x="154" nd="1"/>
+        <i x="175" nd="1"/>
+        <i x="33" nd="1"/>
+        <i x="126" nd="1"/>
+        <i x="41" nd="1"/>
+        <i x="98" nd="1"/>
+        <i x="109" nd="1"/>
+        <i x="118" nd="1"/>
+        <i x="165" nd="1"/>
+        <i x="99" nd="1"/>
+        <i x="105" nd="1"/>
+        <i x="19" nd="1"/>
+        <i x="127" nd="1"/>
+        <i x="29" nd="1"/>
+        <i x="57" nd="1"/>
+        <i x="11" nd="1"/>
+        <i x="145" nd="1"/>
+        <i x="112" nd="1"/>
+        <i x="138" nd="1"/>
+        <i x="149" nd="1"/>
+        <i x="95" nd="1"/>
+        <i x="122" nd="1"/>
+        <i x="89" nd="1"/>
+        <i x="25" nd="1"/>
+        <i x="162" nd="1"/>
+        <i x="4" nd="1"/>
+        <i x="87" nd="1"/>
+        <i x="27" nd="1"/>
+        <i x="58" nd="1"/>
+        <i x="34" nd="1"/>
+        <i x="178" nd="1"/>
+        <i x="16" nd="1"/>
+        <i x="155" nd="1"/>
+        <i x="62" nd="1"/>
+        <i x="150" nd="1"/>
+        <i x="51" nd="1"/>
+        <i x="139" nd="1"/>
+        <i x="176" nd="1"/>
+        <i x="130" nd="1"/>
+        <i x="74" nd="1"/>
+        <i x="90" nd="1"/>
+        <i x="134" nd="1"/>
+        <i x="159" nd="1"/>
+        <i x="120" nd="1"/>
+        <i x="136" nd="1"/>
+        <i x="81" nd="1"/>
+        <i x="47" nd="1"/>
+        <i x="75" nd="1"/>
+        <i x="35" nd="1"/>
+        <i x="174" nd="1"/>
+        <i x="91" nd="1"/>
+        <i x="137" nd="1"/>
+        <i x="166" nd="1"/>
+        <i x="96" nd="1"/>
+        <i x="36" nd="1"/>
+        <i x="140" nd="1"/>
+        <i x="71" nd="1"/>
+        <i x="124" nd="1"/>
+        <i x="123" nd="1"/>
+        <i x="151" nd="1"/>
+        <i x="93" nd="1"/>
+        <i x="8" nd="1"/>
+        <i x="82" nd="1"/>
+        <i x="52" nd="1"/>
+        <i x="160" nd="1"/>
+        <i x="100" nd="1"/>
+        <i x="128" nd="1"/>
+        <i x="119" nd="1"/>
+        <i x="94" nd="1"/>
+        <i x="26" nd="1"/>
+        <i x="101" nd="1"/>
+        <i x="63" nd="1"/>
+        <i x="146" nd="1"/>
+        <i x="110" nd="1"/>
+        <i x="76" nd="1"/>
+        <i x="66" nd="1"/>
+        <i x="3" nd="1"/>
+        <i x="20" nd="1"/>
+        <i x="156" nd="1"/>
+        <i x="9" nd="1"/>
+        <i x="77" nd="1"/>
+        <i x="106" nd="1"/>
+        <i x="177" nd="1"/>
+        <i x="131" nd="1"/>
+        <i x="163" nd="1"/>
+        <i x="60" nd="1"/>
+        <i x="147" nd="1"/>
+        <i x="38" nd="1"/>
+        <i x="113" nd="1"/>
+        <i x="121" nd="1"/>
+        <i x="10" nd="1"/>
+        <i x="157" nd="1"/>
+        <i x="141" nd="1"/>
+        <i x="132" nd="1"/>
+        <i x="115" nd="1"/>
+        <i x="108" nd="1"/>
+        <i x="88" nd="1"/>
+        <i x="56" nd="1"/>
+        <i x="148" nd="1"/>
+        <i x="46" nd="1"/>
+        <i x="111" nd="1"/>
+        <i x="12" nd="1"/>
+        <i x="117" nd="1"/>
+        <i x="135" nd="1"/>
+        <i x="48" nd="1"/>
+        <i x="59" nd="1"/>
+        <i x="84" nd="1"/>
+        <i x="72" nd="1"/>
+        <i x="164" nd="1"/>
+        <i x="30" nd="1"/>
       </items>
     </tabular>
   </data>
@@ -6284,186 +6301,188 @@
   </pivotTables>
   <data>
     <tabular pivotCacheId="2">
-      <items count="179">
+      <items count="181">
         <i x="0" s="1"/>
-        <i x="44" s="1" nd="1"/>
-        <i x="69" s="1" nd="1"/>
-        <i x="64" s="1" nd="1"/>
-        <i x="4" s="1" nd="1"/>
-        <i x="82" s="1" nd="1"/>
-        <i x="168" s="1" nd="1"/>
-        <i x="40" s="1" nd="1"/>
-        <i x="164" s="1" nd="1"/>
-        <i x="54" s="1" nd="1"/>
-        <i x="49" s="1" nd="1"/>
-        <i x="53" s="1" nd="1"/>
-        <i x="120" s="1" nd="1"/>
-        <i x="148" s="1" nd="1"/>
-        <i x="6" s="1" nd="1"/>
-        <i x="172" s="1" nd="1"/>
-        <i x="107" s="1" nd="1"/>
-        <i x="39" s="1" nd="1"/>
-        <i x="22" s="1" nd="1"/>
-        <i x="70" s="1" nd="1"/>
-        <i x="23" s="1" nd="1"/>
-        <i x="73" s="1" nd="1"/>
-        <i x="130" s="1" nd="1"/>
-        <i x="41" s="1" nd="1"/>
-        <i x="94" s="1" nd="1"/>
-        <i x="160" s="1" nd="1"/>
-        <i x="83" s="1" nd="1"/>
-        <i x="108" s="1" nd="1"/>
-        <i x="86" s="1" nd="1"/>
-        <i x="169" s="1" nd="1"/>
-        <i x="12" s="1" nd="1"/>
-        <i x="154" s="1" nd="1"/>
-        <i x="32" s="1" nd="1"/>
-        <i x="57" s="1" nd="1"/>
-        <i x="50" s="1" nd="1"/>
-        <i x="74" s="1" nd="1"/>
-        <i x="119" s="1" nd="1"/>
-        <i x="170" s="1" nd="1"/>
-        <i x="137" s="1" nd="1"/>
-        <i x="112" s="1" nd="1"/>
-        <i x="33" s="1" nd="1"/>
-        <i x="58" s="1" nd="1"/>
-        <i x="109" s="1" nd="1"/>
-        <i x="34" s="1" nd="1"/>
-        <i x="7" s="1" nd="1"/>
-        <i x="87" s="1" nd="1"/>
-        <i x="20" s="1" nd="1"/>
-        <i x="15" s="1" nd="1"/>
-        <i x="75" s="1" nd="1"/>
-        <i x="171" s="1" nd="1"/>
-        <i x="134" s="1" nd="1"/>
-        <i x="76" s="1" nd="1"/>
-        <i x="173" s="1" nd="1"/>
-        <i x="77" s="1" nd="1"/>
-        <i x="45" s="1" nd="1"/>
-        <i x="155" s="1" nd="1"/>
-        <i x="17" s="1" nd="1"/>
-        <i x="24" s="1" nd="1"/>
-        <i x="29" s="1" nd="1"/>
-        <i x="13" s="1" nd="1"/>
-        <i x="149" s="1" nd="1"/>
-        <i x="59" s="1" nd="1"/>
-        <i x="176" s="1" nd="1"/>
-        <i x="35" s="1" nd="1"/>
-        <i x="131" s="1" nd="1"/>
-        <i x="42" s="1" nd="1"/>
-        <i x="101" s="1" nd="1"/>
-        <i x="114" s="1" nd="1"/>
-        <i x="123" s="1" nd="1"/>
-        <i x="166" s="1" nd="1"/>
-        <i x="102" s="1" nd="1"/>
-        <i x="110" s="1" nd="1"/>
-        <i x="18" s="1" nd="1"/>
-        <i x="132" s="1" nd="1"/>
-        <i x="30" s="1" nd="1"/>
-        <i x="150" s="1" nd="1"/>
-        <i x="118" s="1" nd="1"/>
-        <i x="144" s="1" nd="1"/>
-        <i x="95" s="1" nd="1"/>
-        <i x="99" s="1" nd="1"/>
-        <i x="127" s="1" nd="1"/>
-        <i x="92" s="1" nd="1"/>
-        <i x="25" s="1" nd="1"/>
-        <i x="165" s="1" nd="1"/>
-        <i x="2" s="1" nd="1"/>
-        <i x="88" s="1" nd="1"/>
-        <i x="27" s="1" nd="1"/>
-        <i x="60" s="1" nd="1"/>
-        <i x="36" s="1" nd="1"/>
-        <i x="177" s="1" nd="1"/>
-        <i x="156" s="1" nd="1"/>
-        <i x="65" s="1" nd="1"/>
-        <i x="152" s="1" nd="1"/>
-        <i x="55" s="1" nd="1"/>
-        <i x="145" s="1" nd="1"/>
-        <i x="103" s="1" nd="1"/>
-        <i x="135" s="1" nd="1"/>
-        <i x="78" s="1" nd="1"/>
-        <i x="93" s="1" nd="1"/>
-        <i x="138" s="1" nd="1"/>
-        <i x="161" s="1" nd="1"/>
-        <i x="125" s="1" nd="1"/>
-        <i x="139" s="1" nd="1"/>
-        <i x="96" s="1" nd="1"/>
-        <i x="51" s="1" nd="1"/>
-        <i x="79" s="1" nd="1"/>
-        <i x="174" s="1" nd="1"/>
-        <i x="140" s="1" nd="1"/>
-        <i x="37" s="1" nd="1"/>
-        <i x="146" s="1" nd="1"/>
-        <i x="128" s="1" nd="1"/>
-        <i x="153" s="1" nd="1"/>
-        <i x="84" s="1" nd="1"/>
-        <i x="56" s="1" nd="1"/>
-        <i x="162" s="1" nd="1"/>
-        <i x="124" s="1" nd="1"/>
-        <i x="97" s="1" nd="1"/>
-        <i x="26" s="1" nd="1"/>
-        <i x="104" s="1" nd="1"/>
-        <i x="80" s="1" nd="1"/>
-        <i x="71" s="1" nd="1"/>
-        <i x="1" s="1" nd="1"/>
-        <i x="19" s="1" nd="1"/>
-        <i x="8" s="1" nd="1"/>
-        <i x="81" s="1" nd="1"/>
-        <i x="111" s="1" nd="1"/>
-        <i x="63" s="1" nd="1"/>
-        <i x="151" s="1" nd="1"/>
-        <i x="163" s="1" nd="1"/>
-        <i x="9" s="1" nd="1"/>
-        <i x="157" s="1" nd="1"/>
-        <i x="147" s="1" nd="1"/>
-        <i x="121" s="1" nd="1"/>
-        <i x="113" s="1" nd="1"/>
-        <i x="141" s="1" nd="1"/>
-        <i x="175" s="1" nd="1"/>
-        <i x="98" s="1" nd="1"/>
-        <i x="115" s="1" nd="1"/>
-        <i x="89" s="1" nd="1"/>
-        <i x="116" s="1" nd="1"/>
-        <i x="167" s="1" nd="1"/>
-        <i x="61" s="1" nd="1"/>
-        <i x="16" s="1" nd="1"/>
-        <i x="66" s="1" nd="1"/>
-        <i x="14" s="1" nd="1"/>
-        <i x="46" s="1" nd="1"/>
-        <i x="142" s="1" nd="1"/>
-        <i x="136" s="1" nd="1"/>
-        <i x="67" s="1" nd="1"/>
-        <i x="129" s="1" nd="1"/>
-        <i x="105" s="1" nd="1"/>
-        <i x="72" s="1" nd="1"/>
-        <i x="3" s="1" nd="1"/>
-        <i x="178" s="1" nd="1"/>
-        <i x="85" s="1" nd="1"/>
-        <i x="11" s="1" nd="1"/>
-        <i x="158" s="1" nd="1"/>
-        <i x="90" s="1" nd="1"/>
-        <i x="62" s="1" nd="1"/>
-        <i x="100" s="1" nd="1"/>
-        <i x="10" s="1" nd="1"/>
-        <i x="31" s="1" nd="1"/>
-        <i x="21" s="1" nd="1"/>
-        <i x="47" s="1" nd="1"/>
-        <i x="133" s="1" nd="1"/>
-        <i x="106" s="1" nd="1"/>
-        <i x="122" s="1" nd="1"/>
-        <i x="43" s="1" nd="1"/>
-        <i x="143" s="1" nd="1"/>
-        <i x="52" s="1" nd="1"/>
-        <i x="159" s="1" nd="1"/>
-        <i x="48" s="1" nd="1"/>
-        <i x="91" s="1" nd="1"/>
-        <i x="68" s="1" nd="1"/>
-        <i x="126" s="1" nd="1"/>
-        <i x="28" s="1" nd="1"/>
-        <i x="117" s="1" nd="1"/>
-        <i x="38" s="1" nd="1"/>
-        <i x="5" s="1" nd="1"/>
+        <i x="1"/>
+        <i x="2"/>
+        <i x="46" nd="1"/>
+        <i x="71" nd="1"/>
+        <i x="66" nd="1"/>
+        <i x="6" nd="1"/>
+        <i x="84" nd="1"/>
+        <i x="170" nd="1"/>
+        <i x="42" nd="1"/>
+        <i x="166" nd="1"/>
+        <i x="56" nd="1"/>
+        <i x="51" nd="1"/>
+        <i x="55" nd="1"/>
+        <i x="122" nd="1"/>
+        <i x="150" nd="1"/>
+        <i x="8" nd="1"/>
+        <i x="174" nd="1"/>
+        <i x="109" nd="1"/>
+        <i x="41" nd="1"/>
+        <i x="24" nd="1"/>
+        <i x="72" nd="1"/>
+        <i x="25" nd="1"/>
+        <i x="75" nd="1"/>
+        <i x="132" nd="1"/>
+        <i x="43" nd="1"/>
+        <i x="96" nd="1"/>
+        <i x="162" nd="1"/>
+        <i x="85" nd="1"/>
+        <i x="110" nd="1"/>
+        <i x="88" nd="1"/>
+        <i x="171" nd="1"/>
+        <i x="14" nd="1"/>
+        <i x="156" nd="1"/>
+        <i x="34" nd="1"/>
+        <i x="59" nd="1"/>
+        <i x="52" nd="1"/>
+        <i x="76" nd="1"/>
+        <i x="121" nd="1"/>
+        <i x="172" nd="1"/>
+        <i x="139" nd="1"/>
+        <i x="114" nd="1"/>
+        <i x="35" nd="1"/>
+        <i x="60" nd="1"/>
+        <i x="111" nd="1"/>
+        <i x="36" nd="1"/>
+        <i x="9" nd="1"/>
+        <i x="89" nd="1"/>
+        <i x="22" nd="1"/>
+        <i x="17" nd="1"/>
+        <i x="77" nd="1"/>
+        <i x="173" nd="1"/>
+        <i x="136" nd="1"/>
+        <i x="78" nd="1"/>
+        <i x="175" nd="1"/>
+        <i x="79" nd="1"/>
+        <i x="47" nd="1"/>
+        <i x="157" nd="1"/>
+        <i x="19" nd="1"/>
+        <i x="26" nd="1"/>
+        <i x="31" nd="1"/>
+        <i x="15" nd="1"/>
+        <i x="151" nd="1"/>
+        <i x="61" nd="1"/>
+        <i x="178" nd="1"/>
+        <i x="37" nd="1"/>
+        <i x="133" nd="1"/>
+        <i x="44" nd="1"/>
+        <i x="103" nd="1"/>
+        <i x="116" nd="1"/>
+        <i x="125" nd="1"/>
+        <i x="168" nd="1"/>
+        <i x="104" nd="1"/>
+        <i x="112" nd="1"/>
+        <i x="20" nd="1"/>
+        <i x="134" nd="1"/>
+        <i x="32" nd="1"/>
+        <i x="152" nd="1"/>
+        <i x="120" nd="1"/>
+        <i x="146" nd="1"/>
+        <i x="97" nd="1"/>
+        <i x="101" nd="1"/>
+        <i x="129" nd="1"/>
+        <i x="94" nd="1"/>
+        <i x="27" nd="1"/>
+        <i x="167" nd="1"/>
+        <i x="4" nd="1"/>
+        <i x="90" nd="1"/>
+        <i x="29" nd="1"/>
+        <i x="62" nd="1"/>
+        <i x="38" nd="1"/>
+        <i x="179" nd="1"/>
+        <i x="158" nd="1"/>
+        <i x="67" nd="1"/>
+        <i x="154" nd="1"/>
+        <i x="57" nd="1"/>
+        <i x="147" nd="1"/>
+        <i x="105" nd="1"/>
+        <i x="137" nd="1"/>
+        <i x="80" nd="1"/>
+        <i x="95" nd="1"/>
+        <i x="140" nd="1"/>
+        <i x="163" nd="1"/>
+        <i x="127" nd="1"/>
+        <i x="141" nd="1"/>
+        <i x="98" nd="1"/>
+        <i x="53" nd="1"/>
+        <i x="81" nd="1"/>
+        <i x="176" nd="1"/>
+        <i x="142" nd="1"/>
+        <i x="39" nd="1"/>
+        <i x="148" nd="1"/>
+        <i x="130" nd="1"/>
+        <i x="155" nd="1"/>
+        <i x="86" nd="1"/>
+        <i x="58" nd="1"/>
+        <i x="164" nd="1"/>
+        <i x="126" nd="1"/>
+        <i x="99" nd="1"/>
+        <i x="28" nd="1"/>
+        <i x="106" nd="1"/>
+        <i x="82" nd="1"/>
+        <i x="73" nd="1"/>
+        <i x="3" nd="1"/>
+        <i x="21" nd="1"/>
+        <i x="10" nd="1"/>
+        <i x="83" nd="1"/>
+        <i x="113" nd="1"/>
+        <i x="65" nd="1"/>
+        <i x="153" nd="1"/>
+        <i x="165" nd="1"/>
+        <i x="11" nd="1"/>
+        <i x="159" nd="1"/>
+        <i x="149" nd="1"/>
+        <i x="123" nd="1"/>
+        <i x="115" nd="1"/>
+        <i x="143" nd="1"/>
+        <i x="177" nd="1"/>
+        <i x="100" nd="1"/>
+        <i x="117" nd="1"/>
+        <i x="91" nd="1"/>
+        <i x="118" nd="1"/>
+        <i x="169" nd="1"/>
+        <i x="63" nd="1"/>
+        <i x="18" nd="1"/>
+        <i x="68" nd="1"/>
+        <i x="16" nd="1"/>
+        <i x="48" nd="1"/>
+        <i x="144" nd="1"/>
+        <i x="138" nd="1"/>
+        <i x="69" nd="1"/>
+        <i x="131" nd="1"/>
+        <i x="107" nd="1"/>
+        <i x="74" nd="1"/>
+        <i x="5" nd="1"/>
+        <i x="180" nd="1"/>
+        <i x="87" nd="1"/>
+        <i x="13" nd="1"/>
+        <i x="160" nd="1"/>
+        <i x="92" nd="1"/>
+        <i x="64" nd="1"/>
+        <i x="102" nd="1"/>
+        <i x="12" nd="1"/>
+        <i x="33" nd="1"/>
+        <i x="23" nd="1"/>
+        <i x="49" nd="1"/>
+        <i x="135" nd="1"/>
+        <i x="108" nd="1"/>
+        <i x="124" nd="1"/>
+        <i x="45" nd="1"/>
+        <i x="145" nd="1"/>
+        <i x="54" nd="1"/>
+        <i x="161" nd="1"/>
+        <i x="50" nd="1"/>
+        <i x="93" nd="1"/>
+        <i x="70" nd="1"/>
+        <i x="128" nd="1"/>
+        <i x="30" nd="1"/>
+        <i x="119" nd="1"/>
+        <i x="40" nd="1"/>
+        <i x="7" nd="1"/>
       </items>
     </tabular>
   </data>
@@ -6477,8 +6496,9 @@
   </pivotTables>
   <data>
     <tabular pivotCacheId="1">
-      <items count="1">
-        <i x="0" s="1"/>
+      <items count="2">
+        <i x="1" s="1"/>
+        <i x="0" s="1" nd="1"/>
       </items>
     </tabular>
   </data>
@@ -6493,8 +6513,8 @@
   <data>
     <tabular pivotCacheId="2">
       <items count="2">
+        <i x="1"/>
         <i x="0" s="1"/>
-        <i x="1"/>
       </items>
     </tabular>
   </data>
@@ -6890,7 +6910,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6912,7 +6932,7 @@
       </c>
       <c r="F1" s="4">
         <f>MIN($B:$B)</f>
-        <v>1.31871588528156E-2</v>
+        <v>3.24953813105822E-3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -6920,14 +6940,14 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>2.9612287878990201E-2</v>
+        <v>4.0237335488200196E-3</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="4">
         <f>VLOOKUP(MAX($A:$A),$A:$B,2,FALSE)</f>
-        <v>1.31871588528156E-2</v>
+        <v>3.59822763130069E-3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -6935,7 +6955,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>2.06098556518555E-2</v>
+        <v>3.8368329405784598E-3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -6943,7 +6963,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>1.9641065970063199E-2</v>
+        <v>3.6540711298584899E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -6951,7 +6971,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>1.8915496766567199E-2</v>
+        <v>3.5157108213752499E-3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -6959,7 +6979,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>1.8520979210734399E-2</v>
+        <v>3.47778992727399E-3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -6967,7 +6987,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>1.8202744424343099E-2</v>
+        <v>3.41971893794835E-3</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -6975,7 +6995,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>1.7816403880715401E-2</v>
+        <v>3.3973550889640999E-3</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -6983,7 +7003,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>1.7425937578082099E-2</v>
+        <v>3.3917247783392698E-3</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -6991,7 +7011,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>1.71273350715637E-2</v>
+        <v>3.38736246339977E-3</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -6999,7 +7019,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>1.69132873415947E-2</v>
+        <v>3.3852637279778702E-3</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -7007,7 +7027,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>1.6745075583457902E-2</v>
+        <v>3.3826122526079399E-3</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -7015,7 +7035,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>1.65931023657322E-2</v>
+        <v>3.3818443771451699E-3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -7023,7 +7043,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>1.6450785100460101E-2</v>
+        <v>3.37810162454844E-3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -7031,7 +7051,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1">
-        <v>1.6305642202496501E-2</v>
+        <v>3.3748645801097198E-3</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -7039,7 +7059,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1">
-        <v>1.6170406714081799E-2</v>
+        <v>3.3637979067861999E-3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -7047,7 +7067,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="1">
-        <v>1.6063641756772998E-2</v>
+        <v>3.3517221454531002E-3</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -7055,7 +7075,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="1">
-        <v>1.5996532514691401E-2</v>
+        <v>3.3405574504286099E-3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -7063,7 +7083,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1">
-        <v>1.5957765281200399E-2</v>
+        <v>3.3347005955874898E-3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -7071,7 +7091,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="1">
-        <v>1.5917852520942698E-2</v>
+        <v>3.3300472423434301E-3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -7079,7 +7099,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="1">
-        <v>1.58628057688475E-2</v>
+        <v>3.3225200604647398E-3</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -7087,7 +7107,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="1">
-        <v>1.5785096213221501E-2</v>
+        <v>3.3151437528431398E-3</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -7095,7 +7115,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="1">
-        <v>1.5681013464927701E-2</v>
+        <v>3.3030060585588199E-3</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -7103,7 +7123,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="1">
-        <v>1.5545685775577999E-2</v>
+        <v>3.2958749216049901E-3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -7111,7 +7131,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="1">
-        <v>1.53756905347109E-2</v>
+        <v>3.2886802218854401E-3</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -7119,7 +7139,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1">
-        <v>1.5178616158664201E-2</v>
+        <v>3.2848871778696801E-3</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -7127,7 +7147,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="1">
-        <v>1.49705493822694E-2</v>
+        <v>3.2821216154843599E-3</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -7135,7 +7155,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="1">
-        <v>1.47744789719582E-2</v>
+        <v>3.2788882963359399E-3</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -7143,7 +7163,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="1">
-        <v>1.4620117843151099E-2</v>
+        <v>3.2762323971837798E-3</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -7151,7 +7171,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="1">
-        <v>1.4512683264911201E-2</v>
+        <v>3.274105489254E-3</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -7159,7 +7179,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="1">
-        <v>1.44273331388831E-2</v>
+        <v>3.2715781126171398E-3</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -7167,7 +7187,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="1">
-        <v>1.4341021887957999E-2</v>
+        <v>3.26960743404925E-3</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -7175,7 +7195,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="1">
-        <v>1.4250415377318901E-2</v>
+        <v>3.2677173148840701E-3</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -7183,7 +7203,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="1">
-        <v>1.41776716336608E-2</v>
+        <v>3.26554221101105E-3</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -7191,7 +7211,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="1">
-        <v>1.41749801114202E-2</v>
+        <v>3.2639687415212401E-3</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -7199,7 +7219,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="1">
-        <v>1.42765445634723E-2</v>
+        <v>3.2621894497424399E-3</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -7207,7 +7227,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="1">
-        <v>1.4380438253283501E-2</v>
+        <v>3.26066999696195E-3</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -7215,7 +7235,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="1">
-        <v>1.44595960155129E-2</v>
+        <v>3.2594476360827702E-3</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -7223,7 +7243,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="1">
-        <v>1.4564007520675701E-2</v>
+        <v>3.2581689301878201E-3</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -7231,7 +7251,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="1">
-        <v>1.46931242197752E-2</v>
+        <v>3.25711793266237E-3</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -7239,7 +7259,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="1">
-        <v>1.4799563214182901E-2</v>
+        <v>3.2561104744672801E-3</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -7247,7 +7267,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="1">
-        <v>1.48293748497963E-2</v>
+        <v>3.2551663462072598E-3</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -7255,7 +7275,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="1">
-        <v>1.4769732952117901E-2</v>
+        <v>3.2543020788580201E-3</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -7263,7 +7283,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="1">
-        <v>1.4639918692409999E-2</v>
+        <v>3.2534652855247298E-3</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -7271,7 +7291,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="1">
-        <v>1.4463507570326301E-2</v>
+        <v>3.2527185976505301E-3</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -7279,7 +7299,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="1">
-        <v>1.4290274120867299E-2</v>
+        <v>3.2519982196390598E-3</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -7287,7 +7307,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="1">
-        <v>1.41516253352165E-2</v>
+        <v>3.2513260375708298E-3</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -7295,7 +7315,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="1">
-        <v>1.4036305248737301E-2</v>
+        <v>3.2507032155990601E-3</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -7303,7 +7323,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="1">
-        <v>1.39519507065415E-2</v>
+        <v>3.2501004170626402E-3</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -7311,7 +7331,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="1">
-        <v>1.39120882377028E-2</v>
+        <v>3.24953813105822E-3</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -7319,7 +7339,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="1">
-        <v>1.31871588528156E-2</v>
+        <v>3.59822763130069E-3</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -7327,7 +7347,7 @@
         <v>2</v>
       </c>
       <c r="B52" s="1">
-        <v>1.5881391353905202E-2</v>
+        <v>3.3481787145137791E-3</v>
       </c>
     </row>
   </sheetData>
@@ -7348,15 +7368,14 @@
   <dimension ref="A3:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11.28515625" customWidth="1"/>
     <col min="7" max="8" width="7.5703125" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" customWidth="1"/>
@@ -7395,10 +7414,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="1">
-        <v>4.1928980195963819E-2</v>
+        <v>0.2772221380361804</v>
       </c>
       <c r="C6" s="1">
-        <v>4.1928980195963819E-2</v>
+        <v>0.2772221380361804</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -7406,10 +7425,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="1">
-        <v>6.0340686032065639E-2</v>
+        <v>0.51226119048617502</v>
       </c>
       <c r="C7" s="1">
-        <v>6.0340686032065639E-2</v>
+        <v>0.51226119048617502</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -7417,10 +7436,10 @@
         <v>2</v>
       </c>
       <c r="B8" s="1">
-        <v>6.0982940263218349E-2</v>
+        <v>0.33369284981378805</v>
       </c>
       <c r="C8" s="1">
-        <v>6.0982940263218349E-2</v>
+        <v>0.33369284981378805</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -7428,10 +7447,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="1">
-        <v>7.9162700101733194E-2</v>
+        <v>0.10929455532243956</v>
       </c>
       <c r="C9" s="1">
-        <v>7.9162700101733194E-2</v>
+        <v>0.10929455532243956</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -7439,10 +7458,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="1">
-        <v>6.0603826648245256E-2</v>
+        <v>0.30811768341464579</v>
       </c>
       <c r="C10" s="1">
-        <v>6.0603826648245256E-2</v>
+        <v>0.30811768341464579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>